<commit_message>
Added getColumnCount() into spreadsheet importing classes.
</commit_message>
<xml_diff>
--- a/tests/testXlsx.xlsx
+++ b/tests/testXlsx.xlsx
@@ -236,16 +236,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
-    <numFmt numFmtId="166" formatCode="[$-415]GE\nER&quot;al&quot;"/>
-    <numFmt numFmtId="167" formatCode="[$-415]YYYY\-MM\-DD"/>
-    <numFmt numFmtId="168" formatCode="@"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00"/>
-    <numFmt numFmtId="170" formatCode="[$-809]DD/MM/YYYY"/>
-    <numFmt numFmtId="171" formatCode="D\.MM\.YYYY"/>
-    <numFmt numFmtId="172" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$-809]DD/MM/YYYY"/>
+    <numFmt numFmtId="168" formatCode="[$-415]GE\nER&quot;al&quot;"/>
+    <numFmt numFmtId="169" formatCode="[$-415]YYYY\-MM\-DD"/>
+    <numFmt numFmtId="170" formatCode="D\.MM\.YYYY"/>
+    <numFmt numFmtId="171" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -270,19 +269,19 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -339,12 +338,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,27 +356,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -389,11 +384,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -415,13 +410,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E7"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
   </cols>
@@ -437,7 +432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -447,9 +442,8 @@
       <c r="C2" s="2" t="n">
         <v>43833</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -459,13 +453,6 @@
       <c r="C3" s="2" t="n">
         <v>43834</v>
       </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -486,31 +473,31 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="E2:E7 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -518,19 +505,19 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="5" t="n">
         <v>40185</v>
       </c>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="4" t="n">
         <v>48.49</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="4" t="n">
         <v>550060.8</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="4" t="n">
         <v>11343.8</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -541,19 +528,19 @@
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="5" t="n">
         <v>40186</v>
       </c>
-      <c r="D3" s="6" t="n">
+      <c r="D3" s="4" t="n">
         <v>45.98</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="4" t="n">
         <v>236341.18</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="4" t="n">
         <v>5140.09</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -564,19 +551,19 @@
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="5" t="n">
         <v>40187</v>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="D4" s="4" t="n">
         <v>51.33</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="4" t="n">
         <v>422955.71</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="4" t="n">
         <v>8239.93</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -587,19 +574,19 @@
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="5" t="n">
         <v>40188</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="4" t="n">
         <v>83.58</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="4" t="n">
         <v>372950.9</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="4" t="n">
         <v>4462.2</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -610,19 +597,19 @@
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="5" t="n">
         <v>40200</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="4" t="n">
         <v>33.06</v>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="E6" s="4" t="n">
         <v>281118.11</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="4" t="n">
         <v>8503.27</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -633,19 +620,19 @@
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="5" t="n">
         <v>40202</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="4" t="n">
         <v>61.22</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="4" t="n">
         <v>352779.19</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="4" t="n">
         <v>5762.48</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -656,19 +643,19 @@
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="6" t="n">
+      <c r="B8" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="5" t="n">
         <v>40203</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="4" t="n">
         <v>81.16</v>
       </c>
-      <c r="E8" s="6" t="n">
+      <c r="E8" s="4" t="n">
         <v>403985.68</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="4" t="n">
         <v>4977.65</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -679,19 +666,19 @@
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="5" t="n">
         <v>40205</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="4" t="n">
         <v>78.16</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="4" t="n">
         <v>410101.03</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="4" t="n">
         <v>5246.94</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -702,19 +689,19 @@
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="5" t="n">
         <v>40206</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="4" t="n">
         <v>73.66</v>
       </c>
-      <c r="E10" s="6" t="n">
+      <c r="E10" s="4" t="n">
         <v>323727.84</v>
       </c>
-      <c r="F10" s="6" t="n">
+      <c r="F10" s="4" t="n">
         <v>4394.89</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -725,19 +712,19 @@
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="6" t="n">
+      <c r="B11" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="5" t="n">
         <v>40207</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="4" t="n">
         <v>94.68</v>
       </c>
-      <c r="E11" s="6" t="n">
+      <c r="E11" s="4" t="n">
         <v>548623.75</v>
       </c>
-      <c r="F11" s="6" t="n">
+      <c r="F11" s="4" t="n">
         <v>5794.51</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -748,19 +735,19 @@
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="6" t="n">
+      <c r="B12" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="5" t="n">
         <v>40208</v>
       </c>
-      <c r="D12" s="6" t="n">
+      <c r="D12" s="4" t="n">
         <v>71.55</v>
       </c>
-      <c r="E12" s="6" t="n">
+      <c r="E12" s="4" t="n">
         <v>413429.91</v>
       </c>
-      <c r="F12" s="6" t="n">
+      <c r="F12" s="4" t="n">
         <v>5778.2</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -771,19 +758,19 @@
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="n">
+      <c r="B13" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="5" t="n">
         <v>40209</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="4" t="n">
         <v>80.52</v>
       </c>
-      <c r="E13" s="6" t="n">
+      <c r="E13" s="4" t="n">
         <v>324537.82</v>
       </c>
-      <c r="F13" s="6" t="n">
+      <c r="F13" s="4" t="n">
         <v>4030.52</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -794,19 +781,19 @@
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="6" t="n">
+      <c r="B14" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="5" t="n">
         <v>40210</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="4" t="n">
         <v>92.71</v>
       </c>
-      <c r="E14" s="6" t="n">
+      <c r="E14" s="4" t="n">
         <v>473075.07</v>
       </c>
-      <c r="F14" s="6" t="n">
+      <c r="F14" s="4" t="n">
         <v>5102.74</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -817,19 +804,19 @@
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="6" t="n">
+      <c r="B15" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="5" t="n">
         <v>40211</v>
       </c>
-      <c r="D15" s="6" t="n">
+      <c r="D15" s="4" t="n">
         <v>58.86</v>
       </c>
-      <c r="E15" s="6" t="n">
+      <c r="E15" s="4" t="n">
         <v>339724.62</v>
       </c>
-      <c r="F15" s="6" t="n">
+      <c r="F15" s="4" t="n">
         <v>5771.74</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -840,19 +827,19 @@
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="6" t="n">
+      <c r="B16" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="5" t="n">
         <v>40212</v>
       </c>
-      <c r="D16" s="6" t="n">
+      <c r="D16" s="4" t="n">
         <v>70.17</v>
       </c>
-      <c r="E16" s="6" t="n">
+      <c r="E16" s="4" t="n">
         <v>443233.11</v>
       </c>
-      <c r="F16" s="6" t="n">
+      <c r="F16" s="4" t="n">
         <v>6316.56</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -863,19 +850,19 @@
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="6" t="n">
+      <c r="B17" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="C17" s="7" t="n">
+      <c r="C17" s="5" t="n">
         <v>40213</v>
       </c>
-      <c r="D17" s="6" t="n">
+      <c r="D17" s="4" t="n">
         <v>82.71</v>
       </c>
-      <c r="E17" s="6" t="n">
+      <c r="E17" s="4" t="n">
         <v>426391.14</v>
       </c>
-      <c r="F17" s="6" t="n">
+      <c r="F17" s="4" t="n">
         <v>5155.25</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -886,19 +873,19 @@
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="6" t="n">
+      <c r="B18" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="5" t="n">
         <v>40214</v>
       </c>
-      <c r="D18" s="6" t="n">
+      <c r="D18" s="4" t="n">
         <v>60.89</v>
       </c>
-      <c r="E18" s="6" t="n">
+      <c r="E18" s="4" t="n">
         <v>425907.85</v>
       </c>
-      <c r="F18" s="6" t="n">
+      <c r="F18" s="4" t="n">
         <v>6994.71</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -909,19 +896,19 @@
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="6" t="n">
+      <c r="B19" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="C19" s="7" t="n">
+      <c r="C19" s="5" t="n">
         <v>40215</v>
       </c>
-      <c r="D19" s="6" t="n">
+      <c r="D19" s="4" t="n">
         <v>64.22</v>
       </c>
-      <c r="E19" s="6" t="n">
+      <c r="E19" s="4" t="n">
         <v>444124.57</v>
       </c>
-      <c r="F19" s="6" t="n">
+      <c r="F19" s="4" t="n">
         <v>6915.67</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -932,19 +919,19 @@
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="6" t="n">
+      <c r="B20" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="C20" s="7" t="n">
+      <c r="C20" s="5" t="n">
         <v>40216</v>
       </c>
-      <c r="D20" s="6" t="n">
+      <c r="D20" s="4" t="n">
         <v>68.32</v>
       </c>
-      <c r="E20" s="6" t="n">
+      <c r="E20" s="4" t="n">
         <v>353874.01</v>
       </c>
-      <c r="F20" s="6" t="n">
+      <c r="F20" s="4" t="n">
         <v>5179.65</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -970,10 +957,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E2:E7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -993,10 +980,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B48" activeCellId="1" sqref="E2:E7 B48"/>
+      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.1"/>
@@ -1004,89 +991,89 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="6" t="n">
         <v>200000</v>
       </c>
-      <c r="B2" s="8" t="n">
+      <c r="B2" s="6" t="n">
         <v>51</v>
       </c>
-      <c r="C2" s="8" t="n">
+      <c r="C2" s="6" t="n">
         <f aca="false">A2/B2</f>
         <v>3921.56862745098</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="7" t="n">
         <v>40941</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="n">
+      <c r="A3" s="6" t="n">
         <v>200001</v>
       </c>
-      <c r="B3" s="8" t="n">
+      <c r="B3" s="6" t="n">
         <v>52</v>
       </c>
-      <c r="C3" s="8" t="n">
+      <c r="C3" s="6" t="n">
         <f aca="false">A3/B3</f>
         <v>3846.17307692308</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
+      <c r="A4" s="6" t="n">
         <v>200002</v>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="B4" s="6" t="n">
         <v>53</v>
       </c>
-      <c r="C4" s="8" t="n">
+      <c r="C4" s="6" t="n">
         <f aca="false">A4/B4</f>
         <v>3773.62264150943</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="7" t="n">
         <v>40943</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="6" t="n">
         <v>200003</v>
       </c>
-      <c r="B5" s="8" t="n">
+      <c r="B5" s="6" t="n">
         <v>54</v>
       </c>
-      <c r="C5" s="8" t="n">
+      <c r="C5" s="6" t="n">
         <f aca="false">A5/B5</f>
         <v>3703.75925925926</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="7" t="n">
         <v>40944</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1109,123 +1096,123 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O26" activeCellId="1" sqref="E2:E7 O26"/>
+      <selection pane="topLeft" activeCell="O26" activeCellId="0" sqref="O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="11" t="n">
+      <c r="B2" s="10" t="n">
         <v>25569</v>
       </c>
-      <c r="C2" s="10" t="n">
+      <c r="C2" s="9" t="n">
         <v>52.21</v>
       </c>
-      <c r="D2" s="10" t="n">
+      <c r="D2" s="9" t="n">
         <v>1.47</v>
       </c>
-      <c r="E2" s="11" t="n">
+      <c r="E2" s="10" t="n">
         <v>25569</v>
       </c>
       <c r="F2" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B2,$E$2)</f>
         <v>0</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="9" t="n">
         <f aca="false">SUM(F2:F16)</f>
         <v>105</v>
       </c>
-      <c r="I2" s="10" t="n">
+      <c r="I2" s="9" t="n">
         <f aca="false">SUM(D2:D16)</f>
         <v>24.76</v>
       </c>
-      <c r="J2" s="10" t="n">
+      <c r="J2" s="9" t="n">
         <f aca="false">F2*F2</f>
         <v>0</v>
       </c>
-      <c r="K2" s="10" t="n">
+      <c r="K2" s="9" t="n">
         <f aca="false">C2*C2</f>
         <v>2725.8841</v>
       </c>
-      <c r="L2" s="10" t="n">
+      <c r="L2" s="9" t="n">
         <f aca="false">F2*C2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="12" t="n">
+      <c r="B3" s="11" t="n">
         <f aca="false">B2+1</f>
         <v>25570</v>
       </c>
-      <c r="C3" s="10" t="n">
+      <c r="C3" s="9" t="n">
         <v>53.12</v>
       </c>
-      <c r="D3" s="10" t="n">
+      <c r="D3" s="9" t="n">
         <v>1.5</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B3,$E$2)</f>
         <v>1</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="10" t="n">
+      <c r="H3" s="9" t="n">
         <f aca="false">SUM(C2:C16)</f>
         <v>931.17</v>
       </c>
-      <c r="I3" s="10" t="n">
+      <c r="I3" s="9" t="n">
         <f aca="false">SUM(C2:C16)</f>
         <v>931.17</v>
       </c>
-      <c r="J3" s="10" t="n">
+      <c r="J3" s="9" t="n">
         <f aca="false">F3*F3</f>
         <v>1</v>
       </c>
-      <c r="K3" s="10" t="n">
+      <c r="K3" s="9" t="n">
         <f aca="false">C3*C3</f>
         <v>2821.7344</v>
       </c>
-      <c r="L3" s="10" t="n">
+      <c r="L3" s="9" t="n">
         <f aca="false">F3*C3</f>
         <v>53.12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="12" t="n">
+      <c r="B4" s="11" t="n">
         <f aca="false">B3+1</f>
         <v>25571</v>
       </c>
-      <c r="C4" s="10" t="n">
+      <c r="C4" s="9" t="n">
         <v>54.48</v>
       </c>
-      <c r="D4" s="10" t="n">
+      <c r="D4" s="9" t="n">
         <v>1.52</v>
       </c>
       <c r="F4" s="1" t="n">
@@ -1243,28 +1230,28 @@
         <f aca="false">SUM(J18:J32)</f>
         <v>41.0532</v>
       </c>
-      <c r="J4" s="10" t="n">
+      <c r="J4" s="9" t="n">
         <f aca="false">F4*F4</f>
         <v>4</v>
       </c>
-      <c r="K4" s="10" t="n">
+      <c r="K4" s="9" t="n">
         <f aca="false">C4*C4</f>
         <v>2968.0704</v>
       </c>
-      <c r="L4" s="10" t="n">
+      <c r="L4" s="9" t="n">
         <f aca="false">F4*C4</f>
         <v>108.96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="12" t="n">
+      <c r="B5" s="11" t="n">
         <f aca="false">B4+1</f>
         <v>25572</v>
       </c>
-      <c r="C5" s="10" t="n">
+      <c r="C5" s="9" t="n">
         <v>55.84</v>
       </c>
-      <c r="D5" s="10" t="n">
+      <c r="D5" s="9" t="n">
         <v>1.55</v>
       </c>
       <c r="F5" s="1" t="n">
@@ -1282,28 +1269,28 @@
         <f aca="false">SUM(K18:K32)</f>
         <v>58498.5439</v>
       </c>
-      <c r="J5" s="10" t="n">
+      <c r="J5" s="9" t="n">
         <f aca="false">F5*F5</f>
         <v>9</v>
       </c>
-      <c r="K5" s="10" t="n">
+      <c r="K5" s="9" t="n">
         <f aca="false">C5*C5</f>
         <v>3118.1056</v>
       </c>
-      <c r="L5" s="10" t="n">
+      <c r="L5" s="9" t="n">
         <f aca="false">F5*C5</f>
         <v>167.52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="12" t="n">
+      <c r="B6" s="11" t="n">
         <f aca="false">B5+1</f>
         <v>25573</v>
       </c>
-      <c r="C6" s="10" t="n">
+      <c r="C6" s="9" t="n">
         <v>57.2</v>
       </c>
-      <c r="D6" s="10" t="n">
+      <c r="D6" s="9" t="n">
         <v>1.57</v>
       </c>
       <c r="F6" s="1" t="n">
@@ -1321,28 +1308,28 @@
         <f aca="false">SUM(L18:L32)</f>
         <v>1548.2453</v>
       </c>
-      <c r="J6" s="10" t="n">
+      <c r="J6" s="9" t="n">
         <f aca="false">F6*F6</f>
         <v>16</v>
       </c>
-      <c r="K6" s="10" t="n">
+      <c r="K6" s="9" t="n">
         <f aca="false">C6*C6</f>
         <v>3271.84</v>
       </c>
-      <c r="L6" s="10" t="n">
+      <c r="L6" s="9" t="n">
         <f aca="false">F6*C6</f>
         <v>228.8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="12" t="n">
+      <c r="B7" s="11" t="n">
         <f aca="false">B6+1</f>
         <v>25574</v>
       </c>
-      <c r="C7" s="10" t="n">
+      <c r="C7" s="9" t="n">
         <v>58.57</v>
       </c>
-      <c r="D7" s="10" t="n">
+      <c r="D7" s="9" t="n">
         <v>1.6</v>
       </c>
       <c r="F7" s="1" t="n">
@@ -1358,28 +1345,28 @@
       <c r="I7" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="J7" s="10" t="n">
+      <c r="J7" s="9" t="n">
         <f aca="false">F7*F7</f>
         <v>25</v>
       </c>
-      <c r="K7" s="10" t="n">
+      <c r="K7" s="9" t="n">
         <f aca="false">C7*C7</f>
         <v>3430.4449</v>
       </c>
-      <c r="L7" s="10" t="n">
+      <c r="L7" s="9" t="n">
         <f aca="false">F7*C7</f>
         <v>292.85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="12" t="n">
+      <c r="B8" s="11" t="n">
         <f aca="false">B7+1</f>
         <v>25575</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="9" t="n">
         <v>59.93</v>
       </c>
-      <c r="D8" s="10" t="n">
+      <c r="D8" s="9" t="n">
         <v>1.63</v>
       </c>
       <c r="F8" s="1" t="n">
@@ -1397,28 +1384,28 @@
         <f aca="false">(I7*I6-I2*I3)/(I7*I4-I2*I2)</f>
         <v>61.2721865421088</v>
       </c>
-      <c r="J8" s="10" t="n">
+      <c r="J8" s="9" t="n">
         <f aca="false">F8*F8</f>
         <v>36</v>
       </c>
-      <c r="K8" s="10" t="n">
+      <c r="K8" s="9" t="n">
         <f aca="false">C8*C8</f>
         <v>3591.6049</v>
       </c>
-      <c r="L8" s="10" t="n">
+      <c r="L8" s="9" t="n">
         <f aca="false">F8*C8</f>
         <v>359.58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="12" t="n">
+      <c r="B9" s="11" t="n">
         <f aca="false">B8+1</f>
         <v>25576</v>
       </c>
-      <c r="C9" s="10" t="n">
+      <c r="C9" s="9" t="n">
         <v>61.29</v>
       </c>
-      <c r="D9" s="10" t="n">
+      <c r="D9" s="9" t="n">
         <v>1.65</v>
       </c>
       <c r="F9" s="1" t="n">
@@ -1436,56 +1423,56 @@
         <f aca="false">1/I7*I3-I8*1/I7*I2</f>
         <v>-39.0619559188409</v>
       </c>
-      <c r="J9" s="10" t="n">
+      <c r="J9" s="9" t="n">
         <f aca="false">F9*F9</f>
         <v>49</v>
       </c>
-      <c r="K9" s="10" t="n">
+      <c r="K9" s="9" t="n">
         <f aca="false">C9*C9</f>
         <v>3756.4641</v>
       </c>
-      <c r="L9" s="10" t="n">
+      <c r="L9" s="9" t="n">
         <f aca="false">F9*C9</f>
         <v>429.03</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12" t="n">
+      <c r="B10" s="11" t="n">
         <f aca="false">B9+1</f>
         <v>25577</v>
       </c>
-      <c r="C10" s="10" t="n">
+      <c r="C10" s="9" t="n">
         <v>63.11</v>
       </c>
-      <c r="D10" s="10" t="n">
+      <c r="D10" s="9" t="n">
         <v>1.68</v>
       </c>
       <c r="F10" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B10,$E$2)</f>
         <v>8</v>
       </c>
-      <c r="J10" s="10" t="n">
+      <c r="J10" s="9" t="n">
         <f aca="false">F10*F10</f>
         <v>64</v>
       </c>
-      <c r="K10" s="10" t="n">
+      <c r="K10" s="9" t="n">
         <f aca="false">C10*C10</f>
         <v>3982.8721</v>
       </c>
-      <c r="L10" s="10" t="n">
+      <c r="L10" s="9" t="n">
         <f aca="false">F10*C10</f>
         <v>504.88</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="n">
+      <c r="B11" s="11" t="n">
         <f aca="false">B10+1</f>
         <v>25578</v>
       </c>
-      <c r="C11" s="10" t="n">
+      <c r="C11" s="9" t="n">
         <v>64.47</v>
       </c>
-      <c r="D11" s="10" t="n">
+      <c r="D11" s="9" t="n">
         <v>1.7</v>
       </c>
       <c r="F11" s="1" t="n">
@@ -1495,155 +1482,155 @@
       <c r="H11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="10" t="n">
+      <c r="J11" s="9" t="n">
         <f aca="false">F11*F11</f>
         <v>81</v>
       </c>
-      <c r="K11" s="10" t="n">
+      <c r="K11" s="9" t="n">
         <f aca="false">C11*C11</f>
         <v>4156.3809</v>
       </c>
-      <c r="L11" s="10" t="n">
+      <c r="L11" s="9" t="n">
         <f aca="false">F11*C11</f>
         <v>580.23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="n">
+      <c r="B12" s="11" t="n">
         <f aca="false">B11+1</f>
         <v>25579</v>
       </c>
-      <c r="C12" s="10" t="n">
+      <c r="C12" s="9" t="n">
         <v>66.28</v>
       </c>
-      <c r="D12" s="10" t="n">
+      <c r="D12" s="9" t="n">
         <v>1.73</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B12,$E$2)</f>
         <v>10</v>
       </c>
-      <c r="J12" s="10" t="n">
+      <c r="J12" s="9" t="n">
         <f aca="false">F12*F12</f>
         <v>100</v>
       </c>
-      <c r="K12" s="10" t="n">
+      <c r="K12" s="9" t="n">
         <f aca="false">C12*C12</f>
         <v>4393.0384</v>
       </c>
-      <c r="L12" s="10" t="n">
+      <c r="L12" s="9" t="n">
         <f aca="false">F12*C12</f>
         <v>662.8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="n">
+      <c r="B13" s="11" t="n">
         <f aca="false">B12+1</f>
         <v>25580</v>
       </c>
-      <c r="C13" s="10" t="n">
+      <c r="C13" s="9" t="n">
         <v>68.1</v>
       </c>
-      <c r="D13" s="10" t="n">
+      <c r="D13" s="9" t="n">
         <v>1.75</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B13,$E$2)</f>
         <v>11</v>
       </c>
-      <c r="J13" s="10" t="n">
+      <c r="J13" s="9" t="n">
         <f aca="false">F13*F13</f>
         <v>121</v>
       </c>
-      <c r="K13" s="10" t="n">
+      <c r="K13" s="9" t="n">
         <f aca="false">C13*C13</f>
         <v>4637.61</v>
       </c>
-      <c r="L13" s="10" t="n">
+      <c r="L13" s="9" t="n">
         <f aca="false">F13*C13</f>
         <v>749.1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="n">
+      <c r="B14" s="11" t="n">
         <f aca="false">B13+1</f>
         <v>25581</v>
       </c>
-      <c r="C14" s="10" t="n">
+      <c r="C14" s="9" t="n">
         <v>69.92</v>
       </c>
-      <c r="D14" s="10" t="n">
+      <c r="D14" s="9" t="n">
         <v>1.78</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B14,$E$2)</f>
         <v>12</v>
       </c>
-      <c r="J14" s="10" t="n">
+      <c r="J14" s="9" t="n">
         <f aca="false">F14*F14</f>
         <v>144</v>
       </c>
-      <c r="K14" s="10" t="n">
+      <c r="K14" s="9" t="n">
         <f aca="false">C14*C14</f>
         <v>4888.8064</v>
       </c>
-      <c r="L14" s="10" t="n">
+      <c r="L14" s="9" t="n">
         <f aca="false">F14*C14</f>
         <v>839.04</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="n">
+      <c r="B15" s="11" t="n">
         <f aca="false">B14+1</f>
         <v>25582</v>
       </c>
-      <c r="C15" s="10" t="n">
+      <c r="C15" s="9" t="n">
         <v>72.19</v>
       </c>
-      <c r="D15" s="10" t="n">
+      <c r="D15" s="9" t="n">
         <v>1.8</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B15,$E$2)</f>
         <v>13</v>
       </c>
-      <c r="J15" s="10" t="n">
+      <c r="J15" s="9" t="n">
         <f aca="false">F15*F15</f>
         <v>169</v>
       </c>
-      <c r="K15" s="10" t="n">
+      <c r="K15" s="9" t="n">
         <f aca="false">C15*C15</f>
         <v>5211.3961</v>
       </c>
-      <c r="L15" s="10" t="n">
+      <c r="L15" s="9" t="n">
         <f aca="false">F15*C15</f>
         <v>938.47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="n">
+      <c r="B16" s="11" t="n">
         <f aca="false">B15+1</f>
         <v>25583</v>
       </c>
-      <c r="C16" s="10" t="n">
+      <c r="C16" s="9" t="n">
         <v>74.46</v>
       </c>
-      <c r="D16" s="10" t="n">
+      <c r="D16" s="9" t="n">
         <v>1.83</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B16,$E$2)</f>
         <v>14</v>
       </c>
-      <c r="J16" s="10" t="n">
+      <c r="J16" s="9" t="n">
         <f aca="false">F16*F16</f>
         <v>196</v>
       </c>
-      <c r="K16" s="10" t="n">
+      <c r="K16" s="9" t="n">
         <f aca="false">C16*C16</f>
         <v>5544.2916</v>
       </c>
-      <c r="L16" s="10" t="n">
+      <c r="L16" s="9" t="n">
         <f aca="false">F16*C16</f>
         <v>1042.44</v>
       </c>
@@ -1653,7 +1640,7 @@
         <f aca="false">D2*D2</f>
         <v>2.1609</v>
       </c>
-      <c r="K18" s="10" t="n">
+      <c r="K18" s="9" t="n">
         <f aca="false">C2*C2</f>
         <v>2725.8841</v>
       </c>
@@ -1667,7 +1654,7 @@
         <f aca="false">D3*D3</f>
         <v>2.25</v>
       </c>
-      <c r="K19" s="10" t="n">
+      <c r="K19" s="9" t="n">
         <f aca="false">C3*C3</f>
         <v>2821.7344</v>
       </c>
@@ -1681,7 +1668,7 @@
         <f aca="false">D4*D4</f>
         <v>2.3104</v>
       </c>
-      <c r="K20" s="10" t="n">
+      <c r="K20" s="9" t="n">
         <f aca="false">C4*C4</f>
         <v>2968.0704</v>
       </c>
@@ -1695,7 +1682,7 @@
         <f aca="false">D5*D5</f>
         <v>2.4025</v>
       </c>
-      <c r="K21" s="10" t="n">
+      <c r="K21" s="9" t="n">
         <f aca="false">C5*C5</f>
         <v>3118.1056</v>
       </c>
@@ -1709,7 +1696,7 @@
         <f aca="false">D6*D6</f>
         <v>2.4649</v>
       </c>
-      <c r="K22" s="10" t="n">
+      <c r="K22" s="9" t="n">
         <f aca="false">C6*C6</f>
         <v>3271.84</v>
       </c>
@@ -1723,7 +1710,7 @@
         <f aca="false">D7*D7</f>
         <v>2.56</v>
       </c>
-      <c r="K23" s="10" t="n">
+      <c r="K23" s="9" t="n">
         <f aca="false">C7*C7</f>
         <v>3430.4449</v>
       </c>
@@ -1737,7 +1724,7 @@
         <f aca="false">D8*D8</f>
         <v>2.6569</v>
       </c>
-      <c r="K24" s="10" t="n">
+      <c r="K24" s="9" t="n">
         <f aca="false">C8*C8</f>
         <v>3591.6049</v>
       </c>
@@ -1747,19 +1734,19 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="1" t="n">
         <f aca="false">D9*D9</f>
         <v>2.7225</v>
       </c>
-      <c r="K25" s="10" t="n">
+      <c r="K25" s="9" t="n">
         <f aca="false">C9*C9</f>
         <v>3756.4641</v>
       </c>
@@ -1773,7 +1760,7 @@
         <f aca="false">D10*D10</f>
         <v>2.8224</v>
       </c>
-      <c r="K26" s="10" t="n">
+      <c r="K26" s="9" t="n">
         <f aca="false">C10*C10</f>
         <v>3982.8721</v>
       </c>
@@ -1787,7 +1774,7 @@
         <f aca="false">D11*D11</f>
         <v>2.89</v>
       </c>
-      <c r="K27" s="10" t="n">
+      <c r="K27" s="9" t="n">
         <f aca="false">C11*C11</f>
         <v>4156.3809</v>
       </c>
@@ -1801,7 +1788,7 @@
         <f aca="false">D12*D12</f>
         <v>2.9929</v>
       </c>
-      <c r="K28" s="10" t="n">
+      <c r="K28" s="9" t="n">
         <f aca="false">C12*C12</f>
         <v>4393.0384</v>
       </c>
@@ -1815,7 +1802,7 @@
         <f aca="false">D13*D13</f>
         <v>3.0625</v>
       </c>
-      <c r="K29" s="10" t="n">
+      <c r="K29" s="9" t="n">
         <f aca="false">C13*C13</f>
         <v>4637.61</v>
       </c>
@@ -1829,7 +1816,7 @@
         <f aca="false">D14*D14</f>
         <v>3.1684</v>
       </c>
-      <c r="K30" s="10" t="n">
+      <c r="K30" s="9" t="n">
         <f aca="false">C14*C14</f>
         <v>4888.8064</v>
       </c>
@@ -1843,7 +1830,7 @@
         <f aca="false">D15*D15</f>
         <v>3.24</v>
       </c>
-      <c r="K31" s="10" t="n">
+      <c r="K31" s="9" t="n">
         <f aca="false">C15*C15</f>
         <v>5211.3961</v>
       </c>
@@ -1857,7 +1844,7 @@
         <f aca="false">D16*D16</f>
         <v>3.3489</v>
       </c>
-      <c r="K32" s="10" t="n">
+      <c r="K32" s="9" t="n">
         <f aca="false">C16*C16</f>
         <v>5544.2916</v>
       </c>
@@ -1885,10 +1872,10 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E2:E7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3120,10 +3107,10 @@
   <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="1" sqref="E2:E7 H26"/>
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Correction in xlsx test file.
</commit_message>
<xml_diff>
--- a/tests/testXlsx.xlsx
+++ b/tests/testXlsx.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -236,15 +236,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$-809]DD/MM/YYYY"/>
     <numFmt numFmtId="168" formatCode="[$-415]GE\nER&quot;al&quot;"/>
-    <numFmt numFmtId="169" formatCode="[$-415]YYYY\-MM\-DD"/>
-    <numFmt numFmtId="170" formatCode="D\.MM\.YYYY"/>
-    <numFmt numFmtId="171" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="169" formatCode="[$-415]General"/>
+    <numFmt numFmtId="170" formatCode="[$-415]YYYY\-MM\-DD"/>
+    <numFmt numFmtId="171" formatCode="D\.MM\.YYYY"/>
+    <numFmt numFmtId="172" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -343,7 +344,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -372,7 +373,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,11 +389,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -412,11 +417,11 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="A2:C5 D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
   </cols>
@@ -473,10 +478,10 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -957,10 +962,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:C5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -979,11 +984,11 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.1"/>
@@ -1008,17 +1013,17 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
+      <c r="A2" s="7" t="n">
         <v>200000</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="7" t="n">
         <v>51</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="7" t="n">
         <f aca="false">A2/B2</f>
         <v>3921.56862745098</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="8" t="n">
         <v>40941</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1026,33 +1031,33 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
+      <c r="A3" s="7" t="n">
         <v>200001</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="7" t="n">
         <v>52</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="7" t="n">
         <f aca="false">A3/B3</f>
         <v>3846.17307692308</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+      <c r="A4" s="7" t="n">
         <v>200002</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="7" t="n">
         <v>53</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="7" t="n">
         <f aca="false">A4/B4</f>
         <v>3773.62264150943</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="8" t="n">
         <v>40943</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -1060,17 +1065,17 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
+      <c r="A5" s="7" t="n">
         <v>200003</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="7" t="n">
         <v>54</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="7" t="n">
         <f aca="false">A5/B5</f>
         <v>3703.75925925926</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="8" t="n">
         <v>40944</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -1096,123 +1101,123 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O26" activeCellId="0" sqref="O26"/>
+      <selection pane="topLeft" activeCell="O26" activeCellId="1" sqref="A2:C5 O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="10" t="n">
+      <c r="B2" s="11" t="n">
         <v>25569</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="10" t="n">
         <v>52.21</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="D2" s="10" t="n">
         <v>1.47</v>
       </c>
-      <c r="E2" s="10" t="n">
+      <c r="E2" s="11" t="n">
         <v>25569</v>
       </c>
       <c r="F2" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B2,$E$2)</f>
         <v>0</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="9" t="n">
+      <c r="H2" s="10" t="n">
         <f aca="false">SUM(F2:F16)</f>
         <v>105</v>
       </c>
-      <c r="I2" s="9" t="n">
+      <c r="I2" s="10" t="n">
         <f aca="false">SUM(D2:D16)</f>
         <v>24.76</v>
       </c>
-      <c r="J2" s="9" t="n">
+      <c r="J2" s="10" t="n">
         <f aca="false">F2*F2</f>
         <v>0</v>
       </c>
-      <c r="K2" s="9" t="n">
+      <c r="K2" s="10" t="n">
         <f aca="false">C2*C2</f>
         <v>2725.8841</v>
       </c>
-      <c r="L2" s="9" t="n">
+      <c r="L2" s="10" t="n">
         <f aca="false">F2*C2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="12" t="n">
         <f aca="false">B2+1</f>
         <v>25570</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="10" t="n">
         <v>53.12</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="10" t="n">
         <v>1.5</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B3,$E$2)</f>
         <v>1</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="9" t="n">
+      <c r="H3" s="10" t="n">
         <f aca="false">SUM(C2:C16)</f>
         <v>931.17</v>
       </c>
-      <c r="I3" s="9" t="n">
+      <c r="I3" s="10" t="n">
         <f aca="false">SUM(C2:C16)</f>
         <v>931.17</v>
       </c>
-      <c r="J3" s="9" t="n">
+      <c r="J3" s="10" t="n">
         <f aca="false">F3*F3</f>
         <v>1</v>
       </c>
-      <c r="K3" s="9" t="n">
+      <c r="K3" s="10" t="n">
         <f aca="false">C3*C3</f>
         <v>2821.7344</v>
       </c>
-      <c r="L3" s="9" t="n">
+      <c r="L3" s="10" t="n">
         <f aca="false">F3*C3</f>
         <v>53.12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="12" t="n">
         <f aca="false">B3+1</f>
         <v>25571</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="10" t="n">
         <v>54.48</v>
       </c>
-      <c r="D4" s="9" t="n">
+      <c r="D4" s="10" t="n">
         <v>1.52</v>
       </c>
       <c r="F4" s="1" t="n">
@@ -1230,28 +1235,28 @@
         <f aca="false">SUM(J18:J32)</f>
         <v>41.0532</v>
       </c>
-      <c r="J4" s="9" t="n">
+      <c r="J4" s="10" t="n">
         <f aca="false">F4*F4</f>
         <v>4</v>
       </c>
-      <c r="K4" s="9" t="n">
+      <c r="K4" s="10" t="n">
         <f aca="false">C4*C4</f>
         <v>2968.0704</v>
       </c>
-      <c r="L4" s="9" t="n">
+      <c r="L4" s="10" t="n">
         <f aca="false">F4*C4</f>
         <v>108.96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="12" t="n">
         <f aca="false">B4+1</f>
         <v>25572</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="10" t="n">
         <v>55.84</v>
       </c>
-      <c r="D5" s="9" t="n">
+      <c r="D5" s="10" t="n">
         <v>1.55</v>
       </c>
       <c r="F5" s="1" t="n">
@@ -1269,28 +1274,28 @@
         <f aca="false">SUM(K18:K32)</f>
         <v>58498.5439</v>
       </c>
-      <c r="J5" s="9" t="n">
+      <c r="J5" s="10" t="n">
         <f aca="false">F5*F5</f>
         <v>9</v>
       </c>
-      <c r="K5" s="9" t="n">
+      <c r="K5" s="10" t="n">
         <f aca="false">C5*C5</f>
         <v>3118.1056</v>
       </c>
-      <c r="L5" s="9" t="n">
+      <c r="L5" s="10" t="n">
         <f aca="false">F5*C5</f>
         <v>167.52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="11" t="n">
+      <c r="B6" s="12" t="n">
         <f aca="false">B5+1</f>
         <v>25573</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="10" t="n">
         <v>57.2</v>
       </c>
-      <c r="D6" s="9" t="n">
+      <c r="D6" s="10" t="n">
         <v>1.57</v>
       </c>
       <c r="F6" s="1" t="n">
@@ -1308,28 +1313,28 @@
         <f aca="false">SUM(L18:L32)</f>
         <v>1548.2453</v>
       </c>
-      <c r="J6" s="9" t="n">
+      <c r="J6" s="10" t="n">
         <f aca="false">F6*F6</f>
         <v>16</v>
       </c>
-      <c r="K6" s="9" t="n">
+      <c r="K6" s="10" t="n">
         <f aca="false">C6*C6</f>
         <v>3271.84</v>
       </c>
-      <c r="L6" s="9" t="n">
+      <c r="L6" s="10" t="n">
         <f aca="false">F6*C6</f>
         <v>228.8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="11" t="n">
+      <c r="B7" s="12" t="n">
         <f aca="false">B6+1</f>
         <v>25574</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="10" t="n">
         <v>58.57</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="10" t="n">
         <v>1.6</v>
       </c>
       <c r="F7" s="1" t="n">
@@ -1345,28 +1350,28 @@
       <c r="I7" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="J7" s="9" t="n">
+      <c r="J7" s="10" t="n">
         <f aca="false">F7*F7</f>
         <v>25</v>
       </c>
-      <c r="K7" s="9" t="n">
+      <c r="K7" s="10" t="n">
         <f aca="false">C7*C7</f>
         <v>3430.4449</v>
       </c>
-      <c r="L7" s="9" t="n">
+      <c r="L7" s="10" t="n">
         <f aca="false">F7*C7</f>
         <v>292.85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="11" t="n">
+      <c r="B8" s="12" t="n">
         <f aca="false">B7+1</f>
         <v>25575</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="10" t="n">
         <v>59.93</v>
       </c>
-      <c r="D8" s="9" t="n">
+      <c r="D8" s="10" t="n">
         <v>1.63</v>
       </c>
       <c r="F8" s="1" t="n">
@@ -1384,28 +1389,28 @@
         <f aca="false">(I7*I6-I2*I3)/(I7*I4-I2*I2)</f>
         <v>61.2721865421088</v>
       </c>
-      <c r="J8" s="9" t="n">
+      <c r="J8" s="10" t="n">
         <f aca="false">F8*F8</f>
         <v>36</v>
       </c>
-      <c r="K8" s="9" t="n">
+      <c r="K8" s="10" t="n">
         <f aca="false">C8*C8</f>
         <v>3591.6049</v>
       </c>
-      <c r="L8" s="9" t="n">
+      <c r="L8" s="10" t="n">
         <f aca="false">F8*C8</f>
         <v>359.58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="11" t="n">
+      <c r="B9" s="12" t="n">
         <f aca="false">B8+1</f>
         <v>25576</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="10" t="n">
         <v>61.29</v>
       </c>
-      <c r="D9" s="9" t="n">
+      <c r="D9" s="10" t="n">
         <v>1.65</v>
       </c>
       <c r="F9" s="1" t="n">
@@ -1423,56 +1428,56 @@
         <f aca="false">1/I7*I3-I8*1/I7*I2</f>
         <v>-39.0619559188409</v>
       </c>
-      <c r="J9" s="9" t="n">
+      <c r="J9" s="10" t="n">
         <f aca="false">F9*F9</f>
         <v>49</v>
       </c>
-      <c r="K9" s="9" t="n">
+      <c r="K9" s="10" t="n">
         <f aca="false">C9*C9</f>
         <v>3756.4641</v>
       </c>
-      <c r="L9" s="9" t="n">
+      <c r="L9" s="10" t="n">
         <f aca="false">F9*C9</f>
         <v>429.03</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="11" t="n">
+      <c r="B10" s="12" t="n">
         <f aca="false">B9+1</f>
         <v>25577</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="10" t="n">
         <v>63.11</v>
       </c>
-      <c r="D10" s="9" t="n">
+      <c r="D10" s="10" t="n">
         <v>1.68</v>
       </c>
       <c r="F10" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B10,$E$2)</f>
         <v>8</v>
       </c>
-      <c r="J10" s="9" t="n">
+      <c r="J10" s="10" t="n">
         <f aca="false">F10*F10</f>
         <v>64</v>
       </c>
-      <c r="K10" s="9" t="n">
+      <c r="K10" s="10" t="n">
         <f aca="false">C10*C10</f>
         <v>3982.8721</v>
       </c>
-      <c r="L10" s="9" t="n">
+      <c r="L10" s="10" t="n">
         <f aca="false">F10*C10</f>
         <v>504.88</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="11" t="n">
+      <c r="B11" s="12" t="n">
         <f aca="false">B10+1</f>
         <v>25578</v>
       </c>
-      <c r="C11" s="9" t="n">
+      <c r="C11" s="10" t="n">
         <v>64.47</v>
       </c>
-      <c r="D11" s="9" t="n">
+      <c r="D11" s="10" t="n">
         <v>1.7</v>
       </c>
       <c r="F11" s="1" t="n">
@@ -1482,155 +1487,155 @@
       <c r="H11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="9" t="n">
+      <c r="J11" s="10" t="n">
         <f aca="false">F11*F11</f>
         <v>81</v>
       </c>
-      <c r="K11" s="9" t="n">
+      <c r="K11" s="10" t="n">
         <f aca="false">C11*C11</f>
         <v>4156.3809</v>
       </c>
-      <c r="L11" s="9" t="n">
+      <c r="L11" s="10" t="n">
         <f aca="false">F11*C11</f>
         <v>580.23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="11" t="n">
+      <c r="B12" s="12" t="n">
         <f aca="false">B11+1</f>
         <v>25579</v>
       </c>
-      <c r="C12" s="9" t="n">
+      <c r="C12" s="10" t="n">
         <v>66.28</v>
       </c>
-      <c r="D12" s="9" t="n">
+      <c r="D12" s="10" t="n">
         <v>1.73</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B12,$E$2)</f>
         <v>10</v>
       </c>
-      <c r="J12" s="9" t="n">
+      <c r="J12" s="10" t="n">
         <f aca="false">F12*F12</f>
         <v>100</v>
       </c>
-      <c r="K12" s="9" t="n">
+      <c r="K12" s="10" t="n">
         <f aca="false">C12*C12</f>
         <v>4393.0384</v>
       </c>
-      <c r="L12" s="9" t="n">
+      <c r="L12" s="10" t="n">
         <f aca="false">F12*C12</f>
         <v>662.8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="11" t="n">
+      <c r="B13" s="12" t="n">
         <f aca="false">B12+1</f>
         <v>25580</v>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="10" t="n">
         <v>68.1</v>
       </c>
-      <c r="D13" s="9" t="n">
+      <c r="D13" s="10" t="n">
         <v>1.75</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B13,$E$2)</f>
         <v>11</v>
       </c>
-      <c r="J13" s="9" t="n">
+      <c r="J13" s="10" t="n">
         <f aca="false">F13*F13</f>
         <v>121</v>
       </c>
-      <c r="K13" s="9" t="n">
+      <c r="K13" s="10" t="n">
         <f aca="false">C13*C13</f>
         <v>4637.61</v>
       </c>
-      <c r="L13" s="9" t="n">
+      <c r="L13" s="10" t="n">
         <f aca="false">F13*C13</f>
         <v>749.1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="11" t="n">
+      <c r="B14" s="12" t="n">
         <f aca="false">B13+1</f>
         <v>25581</v>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="10" t="n">
         <v>69.92</v>
       </c>
-      <c r="D14" s="9" t="n">
+      <c r="D14" s="10" t="n">
         <v>1.78</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B14,$E$2)</f>
         <v>12</v>
       </c>
-      <c r="J14" s="9" t="n">
+      <c r="J14" s="10" t="n">
         <f aca="false">F14*F14</f>
         <v>144</v>
       </c>
-      <c r="K14" s="9" t="n">
+      <c r="K14" s="10" t="n">
         <f aca="false">C14*C14</f>
         <v>4888.8064</v>
       </c>
-      <c r="L14" s="9" t="n">
+      <c r="L14" s="10" t="n">
         <f aca="false">F14*C14</f>
         <v>839.04</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="11" t="n">
+      <c r="B15" s="12" t="n">
         <f aca="false">B14+1</f>
         <v>25582</v>
       </c>
-      <c r="C15" s="9" t="n">
+      <c r="C15" s="10" t="n">
         <v>72.19</v>
       </c>
-      <c r="D15" s="9" t="n">
+      <c r="D15" s="10" t="n">
         <v>1.8</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B15,$E$2)</f>
         <v>13</v>
       </c>
-      <c r="J15" s="9" t="n">
+      <c r="J15" s="10" t="n">
         <f aca="false">F15*F15</f>
         <v>169</v>
       </c>
-      <c r="K15" s="9" t="n">
+      <c r="K15" s="10" t="n">
         <f aca="false">C15*C15</f>
         <v>5211.3961</v>
       </c>
-      <c r="L15" s="9" t="n">
+      <c r="L15" s="10" t="n">
         <f aca="false">F15*C15</f>
         <v>938.47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="11" t="n">
+      <c r="B16" s="12" t="n">
         <f aca="false">B15+1</f>
         <v>25583</v>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="C16" s="10" t="n">
         <v>74.46</v>
       </c>
-      <c r="D16" s="9" t="n">
+      <c r="D16" s="10" t="n">
         <v>1.83</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B16,$E$2)</f>
         <v>14</v>
       </c>
-      <c r="J16" s="9" t="n">
+      <c r="J16" s="10" t="n">
         <f aca="false">F16*F16</f>
         <v>196</v>
       </c>
-      <c r="K16" s="9" t="n">
+      <c r="K16" s="10" t="n">
         <f aca="false">C16*C16</f>
         <v>5544.2916</v>
       </c>
-      <c r="L16" s="9" t="n">
+      <c r="L16" s="10" t="n">
         <f aca="false">F16*C16</f>
         <v>1042.44</v>
       </c>
@@ -1640,7 +1645,7 @@
         <f aca="false">D2*D2</f>
         <v>2.1609</v>
       </c>
-      <c r="K18" s="9" t="n">
+      <c r="K18" s="10" t="n">
         <f aca="false">C2*C2</f>
         <v>2725.8841</v>
       </c>
@@ -1654,7 +1659,7 @@
         <f aca="false">D3*D3</f>
         <v>2.25</v>
       </c>
-      <c r="K19" s="9" t="n">
+      <c r="K19" s="10" t="n">
         <f aca="false">C3*C3</f>
         <v>2821.7344</v>
       </c>
@@ -1668,7 +1673,7 @@
         <f aca="false">D4*D4</f>
         <v>2.3104</v>
       </c>
-      <c r="K20" s="9" t="n">
+      <c r="K20" s="10" t="n">
         <f aca="false">C4*C4</f>
         <v>2968.0704</v>
       </c>
@@ -1682,7 +1687,7 @@
         <f aca="false">D5*D5</f>
         <v>2.4025</v>
       </c>
-      <c r="K21" s="9" t="n">
+      <c r="K21" s="10" t="n">
         <f aca="false">C5*C5</f>
         <v>3118.1056</v>
       </c>
@@ -1696,7 +1701,7 @@
         <f aca="false">D6*D6</f>
         <v>2.4649</v>
       </c>
-      <c r="K22" s="9" t="n">
+      <c r="K22" s="10" t="n">
         <f aca="false">C6*C6</f>
         <v>3271.84</v>
       </c>
@@ -1710,7 +1715,7 @@
         <f aca="false">D7*D7</f>
         <v>2.56</v>
       </c>
-      <c r="K23" s="9" t="n">
+      <c r="K23" s="10" t="n">
         <f aca="false">C7*C7</f>
         <v>3430.4449</v>
       </c>
@@ -1724,7 +1729,7 @@
         <f aca="false">D8*D8</f>
         <v>2.6569</v>
       </c>
-      <c r="K24" s="9" t="n">
+      <c r="K24" s="10" t="n">
         <f aca="false">C8*C8</f>
         <v>3591.6049</v>
       </c>
@@ -1734,19 +1739,19 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
       <c r="J25" s="1" t="n">
         <f aca="false">D9*D9</f>
         <v>2.7225</v>
       </c>
-      <c r="K25" s="9" t="n">
+      <c r="K25" s="10" t="n">
         <f aca="false">C9*C9</f>
         <v>3756.4641</v>
       </c>
@@ -1760,7 +1765,7 @@
         <f aca="false">D10*D10</f>
         <v>2.8224</v>
       </c>
-      <c r="K26" s="9" t="n">
+      <c r="K26" s="10" t="n">
         <f aca="false">C10*C10</f>
         <v>3982.8721</v>
       </c>
@@ -1774,7 +1779,7 @@
         <f aca="false">D11*D11</f>
         <v>2.89</v>
       </c>
-      <c r="K27" s="9" t="n">
+      <c r="K27" s="10" t="n">
         <f aca="false">C11*C11</f>
         <v>4156.3809</v>
       </c>
@@ -1788,7 +1793,7 @@
         <f aca="false">D12*D12</f>
         <v>2.9929</v>
       </c>
-      <c r="K28" s="9" t="n">
+      <c r="K28" s="10" t="n">
         <f aca="false">C12*C12</f>
         <v>4393.0384</v>
       </c>
@@ -1802,7 +1807,7 @@
         <f aca="false">D13*D13</f>
         <v>3.0625</v>
       </c>
-      <c r="K29" s="9" t="n">
+      <c r="K29" s="10" t="n">
         <f aca="false">C13*C13</f>
         <v>4637.61</v>
       </c>
@@ -1816,7 +1821,7 @@
         <f aca="false">D14*D14</f>
         <v>3.1684</v>
       </c>
-      <c r="K30" s="9" t="n">
+      <c r="K30" s="10" t="n">
         <f aca="false">C14*C14</f>
         <v>4888.8064</v>
       </c>
@@ -1830,7 +1835,7 @@
         <f aca="false">D15*D15</f>
         <v>3.24</v>
       </c>
-      <c r="K31" s="9" t="n">
+      <c r="K31" s="10" t="n">
         <f aca="false">C15*C15</f>
         <v>5211.3961</v>
       </c>
@@ -1844,7 +1849,7 @@
         <f aca="false">D16*D16</f>
         <v>3.3489</v>
       </c>
-      <c r="K32" s="9" t="n">
+      <c r="K32" s="10" t="n">
         <f aca="false">C16*C16</f>
         <v>5544.2916</v>
       </c>
@@ -1872,10 +1877,10 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:C5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3107,10 +3112,10 @@
   <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+      <selection pane="topLeft" activeCell="H26" activeCellId="1" sqref="A2:C5 H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Truncated 6th and 7th xlsx test sheet. Added compare data for 5th, 6th and th sheet.
</commit_message>
<xml_diff>
--- a/tests/testXlsx.xlsx
+++ b/tests/testXlsx.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -242,7 +242,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$-809]DD/MM/YYYY"/>
     <numFmt numFmtId="168" formatCode="[$-415]GE\nER&quot;al&quot;"/>
-    <numFmt numFmtId="169" formatCode="[$-415]General"/>
+    <numFmt numFmtId="169" formatCode="[$-415]GE\nER&quot;al&quot;"/>
     <numFmt numFmtId="170" formatCode="[$-415]YYYY\-MM\-DD"/>
     <numFmt numFmtId="171" formatCode="D\.MM\.YYYY"/>
     <numFmt numFmtId="172" formatCode="DD/MM/YY"/>
@@ -418,10 +418,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="A2:C5 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
   </cols>
@@ -478,10 +478,14 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="A2:C5"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.39"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -962,10 +966,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -984,11 +988,11 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.1"/>
@@ -1101,10 +1105,13 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O26" activeCellId="1" sqref="A2:C5 O26"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.58"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1874,13 +1881,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:C5 A1"/>
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2191,906 +2198,6 @@
       </c>
       <c r="C26" s="1" t="n">
         <v>0.174372</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="B27" s="1" t="n">
-        <f aca="false">C27*71</f>
-        <v>12.478037</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>0.175747</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="B28" s="1" t="n">
-        <f aca="false">C28*71</f>
-        <v>12.55138</v>
-      </c>
-      <c r="C28" s="1" t="n">
-        <v>0.17678</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="B29" s="1" t="n">
-        <f aca="false">C29*71</f>
-        <v>12.600157</v>
-      </c>
-      <c r="C29" s="1" t="n">
-        <v>0.177467</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="B30" s="1" t="n">
-        <f aca="false">C30*71</f>
-        <v>12.623942</v>
-      </c>
-      <c r="C30" s="1" t="n">
-        <v>0.177802</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="B31" s="1" t="n">
-        <f aca="false">C31*71</f>
-        <v>12.622735</v>
-      </c>
-      <c r="C31" s="1" t="n">
-        <v>0.177785</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B32" s="1" t="n">
-        <f aca="false">C32*71</f>
-        <v>12.596465</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>0.177415</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="B33" s="1" t="n">
-        <f aca="false">C33*71</f>
-        <v>12.545274</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <v>0.176694</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="B34" s="1" t="n">
-        <f aca="false">C34*71</f>
-        <v>12.469446</v>
-      </c>
-      <c r="C34" s="1" t="n">
-        <v>0.175626</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="B35" s="1" t="n">
-        <f aca="false">C35*71</f>
-        <v>12.369549</v>
-      </c>
-      <c r="C35" s="1" t="n">
-        <v>0.174219</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="B36" s="1" t="n">
-        <f aca="false">C36*71</f>
-        <v>12.246009</v>
-      </c>
-      <c r="C36" s="1" t="n">
-        <v>0.172479</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="B37" s="1" t="n">
-        <f aca="false">C37*71</f>
-        <v>12.099678</v>
-      </c>
-      <c r="C37" s="1" t="n">
-        <v>0.170418</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="B38" s="1" t="n">
-        <f aca="false">C38*71</f>
-        <v>11.931408</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>0.168048</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="B39" s="1" t="n">
-        <f aca="false">C39*71</f>
-        <v>11.742051</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <v>0.165381</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="B40" s="1" t="n">
-        <f aca="false">C40*71</f>
-        <v>11.532814</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <v>0.162434</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="B41" s="1" t="n">
-        <f aca="false">C41*71</f>
-        <v>11.304762</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>0.159222</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B42" s="1" t="n">
-        <f aca="false">C42*71</f>
-        <v>11.059315</v>
-      </c>
-      <c r="C42" s="1" t="n">
-        <v>0.155765</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="B43" s="1" t="n">
-        <f aca="false">C43*71</f>
-        <v>10.797609</v>
-      </c>
-      <c r="C43" s="1" t="n">
-        <v>0.152079</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="B44" s="1" t="n">
-        <f aca="false">C44*71</f>
-        <v>10.521206</v>
-      </c>
-      <c r="C44" s="1" t="n">
-        <v>0.148186</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="B45" s="1" t="n">
-        <f aca="false">C45*71</f>
-        <v>10.231597</v>
-      </c>
-      <c r="C45" s="1" t="n">
-        <v>0.144107</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="B46" s="1" t="n">
-        <f aca="false">C46*71</f>
-        <v>9.930131</v>
-      </c>
-      <c r="C46" s="1" t="n">
-        <v>0.139861</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="B47" s="1" t="n">
-        <f aca="false">C47*71</f>
-        <v>9.618441</v>
-      </c>
-      <c r="C47" s="1" t="n">
-        <v>0.135471</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="B48" s="1" t="n">
-        <f aca="false">C48*71</f>
-        <v>9.298018</v>
-      </c>
-      <c r="C48" s="1" t="n">
-        <v>0.130958</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="B49" s="1" t="n">
-        <f aca="false">C49*71</f>
-        <v>8.970424</v>
-      </c>
-      <c r="C49" s="1" t="n">
-        <v>0.126344</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="B50" s="1" t="n">
-        <f aca="false">C50*71</f>
-        <v>8.637221</v>
-      </c>
-      <c r="C50" s="1" t="n">
-        <v>0.121651</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="B51" s="1" t="n">
-        <f aca="false">C51*71</f>
-        <v>8.2999</v>
-      </c>
-      <c r="C51" s="1" t="n">
-        <v>0.1169</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B52" s="1" t="n">
-        <f aca="false">C52*71</f>
-        <v>7.959881</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <v>0.112111</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="B53" s="1" t="n">
-        <f aca="false">C53*71</f>
-        <v>7.618655</v>
-      </c>
-      <c r="C53" s="1" t="n">
-        <v>0.107305</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="B54" s="1" t="n">
-        <f aca="false">C54*71</f>
-        <v>7.277571</v>
-      </c>
-      <c r="C54" s="1" t="n">
-        <v>0.102501</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
-        <v>5.3</v>
-      </c>
-      <c r="B55" s="1" t="n">
-        <f aca="false">C55*71</f>
-        <v>6.9379425</v>
-      </c>
-      <c r="C55" s="1" t="n">
-        <v>0.0977175</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="B56" s="1" t="n">
-        <f aca="false">C56*71</f>
-        <v>6.6010475</v>
-      </c>
-      <c r="C56" s="1" t="n">
-        <v>0.0929725</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="B57" s="1" t="n">
-        <f aca="false">C57*71</f>
-        <v>6.2680433</v>
-      </c>
-      <c r="C57" s="1" t="n">
-        <v>0.0882823</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="B58" s="1" t="n">
-        <f aca="false">C58*71</f>
-        <v>5.9400304</v>
-      </c>
-      <c r="C58" s="1" t="n">
-        <v>0.0836624</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="B59" s="1" t="n">
-        <f aca="false">C59*71</f>
-        <v>5.6180028</v>
-      </c>
-      <c r="C59" s="1" t="n">
-        <v>0.0791268</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="B60" s="1" t="n">
-        <f aca="false">C60*71</f>
-        <v>5.3028835</v>
-      </c>
-      <c r="C60" s="1" t="n">
-        <v>0.0746885</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="B61" s="1" t="n">
-        <f aca="false">C61*71</f>
-        <v>4.9955032</v>
-      </c>
-      <c r="C61" s="1" t="n">
-        <v>0.0703592</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B62" s="1" t="n">
-        <f aca="false">C62*71</f>
-        <v>4.6966003</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <v>0.0661493</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="B63" s="1" t="n">
-        <f aca="false">C63*71</f>
-        <v>4.4068138</v>
-      </c>
-      <c r="C63" s="1" t="n">
-        <v>0.0620678</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="B64" s="1" t="n">
-        <f aca="false">C64*71</f>
-        <v>4.1267046</v>
-      </c>
-      <c r="C64" s="1" t="n">
-        <v>0.0581226</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="B65" s="1" t="n">
-        <f aca="false">C65*71</f>
-        <v>3.85672</v>
-      </c>
-      <c r="C65" s="1" t="n">
-        <v>0.05432</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="B66" s="1" t="n">
-        <f aca="false">C66*71</f>
-        <v>3.5972505</v>
-      </c>
-      <c r="C66" s="1" t="n">
-        <v>0.0506655</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="B67" s="1" t="n">
-        <f aca="false">C67*71</f>
-        <v>3.348573</v>
-      </c>
-      <c r="C67" s="1" t="n">
-        <v>0.047163</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="n">
-        <v>6.6</v>
-      </c>
-      <c r="B68" s="1" t="n">
-        <f aca="false">C68*71</f>
-        <v>3.1109005</v>
-      </c>
-      <c r="C68" s="1" t="n">
-        <v>0.0438155</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="B69" s="1" t="n">
-        <f aca="false">C69*71</f>
-        <v>2.8843608</v>
-      </c>
-      <c r="C69" s="1" t="n">
-        <v>0.0406248</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="n">
-        <v>6.8</v>
-      </c>
-      <c r="B70" s="1" t="n">
-        <f aca="false">C70*71</f>
-        <v>2.6690036</v>
-      </c>
-      <c r="C70" s="1" t="n">
-        <v>0.0375916</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="B71" s="1" t="n">
-        <f aca="false">C71*71</f>
-        <v>2.4648289</v>
-      </c>
-      <c r="C71" s="1" t="n">
-        <v>0.0347159</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B72" s="1" t="n">
-        <f aca="false">C72*71</f>
-        <v>2.2717515</v>
-      </c>
-      <c r="C72" s="1" t="n">
-        <v>0.0319965</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="n">
-        <v>7.1</v>
-      </c>
-      <c r="B73" s="1" t="n">
-        <f aca="false">C73*71</f>
-        <v>2.0896436</v>
-      </c>
-      <c r="C73" s="1" t="n">
-        <v>0.0294316</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="B74" s="1" t="n">
-        <f aca="false">C74*71</f>
-        <v>1.9183206</v>
-      </c>
-      <c r="C74" s="1" t="n">
-        <v>0.0270186</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
-        <v>7.3</v>
-      </c>
-      <c r="B75" s="1" t="n">
-        <f aca="false">C75*71</f>
-        <v>1.7575411</v>
-      </c>
-      <c r="C75" s="1" t="n">
-        <v>0.0247541</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="B76" s="1" t="n">
-        <f aca="false">C76*71</f>
-        <v>1.6070424</v>
-      </c>
-      <c r="C76" s="1" t="n">
-        <v>0.0226344</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="B77" s="1" t="n">
-        <f aca="false">C77*71</f>
-        <v>1.4665192</v>
-      </c>
-      <c r="C77" s="1" t="n">
-        <v>0.0206552</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="n">
-        <v>7.6</v>
-      </c>
-      <c r="B78" s="1" t="n">
-        <f aca="false">C78*71</f>
-        <v>1.3356236</v>
-      </c>
-      <c r="C78" s="1" t="n">
-        <v>0.0188116</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="B79" s="1" t="n">
-        <f aca="false">C79*71</f>
-        <v>1.2139935</v>
-      </c>
-      <c r="C79" s="1" t="n">
-        <v>0.0170985</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="n">
-        <v>7.79999</v>
-      </c>
-      <c r="B80" s="1" t="n">
-        <f aca="false">C80*71</f>
-        <v>1.1012526</v>
-      </c>
-      <c r="C80" s="1" t="n">
-        <v>0.0155106</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="n">
-        <v>7.89999</v>
-      </c>
-      <c r="B81" s="1" t="n">
-        <f aca="false">C81*71</f>
-        <v>0.9969962</v>
-      </c>
-      <c r="C81" s="1" t="n">
-        <v>0.0140422</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="n">
-        <v>7.99999</v>
-      </c>
-      <c r="B82" s="1" t="n">
-        <f aca="false">C82*71</f>
-        <v>0.9008196</v>
-      </c>
-      <c r="C82" s="1" t="n">
-        <v>0.0126876</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="n">
-        <v>8.09999</v>
-      </c>
-      <c r="B83" s="1" t="n">
-        <f aca="false">C83*71</f>
-        <v>0.8123039</v>
-      </c>
-      <c r="C83" s="1" t="n">
-        <v>0.0114409</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="B84" s="1" t="n">
-        <f aca="false">C84*71</f>
-        <v>0.7310302</v>
-      </c>
-      <c r="C84" s="1" t="n">
-        <v>0.0102962</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="n">
-        <v>8.3</v>
-      </c>
-      <c r="B85" s="1" t="n">
-        <f aca="false">C85*71</f>
-        <v>0.65658599</v>
-      </c>
-      <c r="C85" s="1" t="n">
-        <v>0.00924769</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
-        <v>8.4</v>
-      </c>
-      <c r="B86" s="1" t="n">
-        <f aca="false">C86*71</f>
-        <v>0.58855024</v>
-      </c>
-      <c r="C86" s="1" t="n">
-        <v>0.00828944</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="B87" s="1" t="n">
-        <f aca="false">C87*71</f>
-        <v>0.52651683</v>
-      </c>
-      <c r="C87" s="1" t="n">
-        <v>0.00741573</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="B88" s="1" t="n">
-        <f aca="false">C88*71</f>
-        <v>0.47008745</v>
-      </c>
-      <c r="C88" s="1" t="n">
-        <v>0.00662095</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="n">
-        <v>8.7</v>
-      </c>
-      <c r="B89" s="1" t="n">
-        <f aca="false">C89*71</f>
-        <v>0.4188716</v>
-      </c>
-      <c r="C89" s="1" t="n">
-        <v>0.0058996</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="n">
-        <v>8.8</v>
-      </c>
-      <c r="B90" s="1" t="n">
-        <f aca="false">C90*71</f>
-        <v>0.37249582</v>
-      </c>
-      <c r="C90" s="1" t="n">
-        <v>0.00524642</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="n">
-        <v>8.9</v>
-      </c>
-      <c r="B91" s="1" t="n">
-        <f aca="false">C91*71</f>
-        <v>0.33059588</v>
-      </c>
-      <c r="C91" s="1" t="n">
-        <v>0.00465628</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B92" s="1" t="n">
-        <f aca="false">C92*71</f>
-        <v>0.29282743</v>
-      </c>
-      <c r="C92" s="1" t="n">
-        <v>0.00412433</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="n">
-        <v>9.1</v>
-      </c>
-      <c r="B93" s="1" t="n">
-        <f aca="false">C93*71</f>
-        <v>0.25885819</v>
-      </c>
-      <c r="C93" s="1" t="n">
-        <v>0.00364589</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="n">
-        <v>9.2</v>
-      </c>
-      <c r="B94" s="1" t="n">
-        <f aca="false">C94*71</f>
-        <v>0.22837576</v>
-      </c>
-      <c r="C94" s="1" t="n">
-        <v>0.00321656</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="n">
-        <v>9.3</v>
-      </c>
-      <c r="B95" s="1" t="n">
-        <f aca="false">C95*71</f>
-        <v>0.20108265</v>
-      </c>
-      <c r="C95" s="1" t="n">
-        <v>0.00283215</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="n">
-        <v>9.4</v>
-      </c>
-      <c r="B96" s="1" t="n">
-        <f aca="false">C96*71</f>
-        <v>0.17669983</v>
-      </c>
-      <c r="C96" s="1" t="n">
-        <v>0.00248873</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="B97" s="1" t="n">
-        <f aca="false">C97*71</f>
-        <v>0.15496531</v>
-      </c>
-      <c r="C97" s="1" t="n">
-        <v>0.00218261</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="n">
-        <v>9.6</v>
-      </c>
-      <c r="B98" s="1" t="n">
-        <f aca="false">C98*71</f>
-        <v>0.13563485</v>
-      </c>
-      <c r="C98" s="1" t="n">
-        <v>0.00191035</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="n">
-        <v>9.7</v>
-      </c>
-      <c r="B99" s="1" t="n">
-        <f aca="false">C99*71</f>
-        <v>0.11847983</v>
-      </c>
-      <c r="C99" s="1" t="n">
-        <v>0.00166873</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="n">
-        <v>9.8</v>
-      </c>
-      <c r="B100" s="1" t="n">
-        <f aca="false">C100*71</f>
-        <v>0.10328867</v>
-      </c>
-      <c r="C100" s="1" t="n">
-        <v>0.00145477</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="n">
-        <v>9.9</v>
-      </c>
-      <c r="B101" s="1" t="n">
-        <f aca="false">C101*71</f>
-        <v>0.08986683</v>
-      </c>
-      <c r="C101" s="1" t="n">
-        <v>0.00126573</v>
       </c>
     </row>
   </sheetData>
@@ -3109,13 +2216,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="1" sqref="A2:C5 H26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3143,8 +2250,8 @@
         <v>61</v>
       </c>
       <c r="F2" s="1" t="n">
-        <f aca="false">AVERAGE(C2:C72)</f>
-        <v>7160.98075109542</v>
+        <f aca="false">AVERAGE(C2:C21)</f>
+        <v>6715.2873295802</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3162,8 +2269,8 @@
         <v>62</v>
       </c>
       <c r="F3" s="1" t="n">
-        <f aca="false">_xlfn.QUARTILE.INC(C$2:C$72,2)</f>
-        <v>6566.64705882353</v>
+        <f aca="false">_xlfn.QUARTILE.INC(C$2:C$21,2)</f>
+        <v>6277.77777777778</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3181,8 +2288,8 @@
         <v>63</v>
       </c>
       <c r="F4" s="1" t="n">
-        <f aca="false">_xlfn.PERCENTILE.INC(C$2:C$72,0.1)</f>
-        <v>4119.16363636364</v>
+        <f aca="false">_xlfn.PERCENTILE.INC(C$2:C$21,0.1)</f>
+        <v>4301.1655011655</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3200,8 +2307,8 @@
         <v>64</v>
       </c>
       <c r="F5" s="1" t="n">
-        <f aca="false">_xlfn.PERCENTILE.INC(C$2:C$72,0.25)</f>
-        <v>5017.38888888889</v>
+        <f aca="false">_xlfn.PERCENTILE.INC(C$2:C$21,0.25)</f>
+        <v>5065.78947368422</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3219,8 +2326,8 @@
         <v>65</v>
       </c>
       <c r="F6" s="1" t="n">
-        <f aca="false">_xlfn.PERCENTILE.INC(C$2:C$72,0.5)</f>
-        <v>6566.64705882353</v>
+        <f aca="false">_xlfn.PERCENTILE.INC(C$2:C$21,0.5)</f>
+        <v>6277.77777777778</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3238,8 +2345,8 @@
         <v>66</v>
       </c>
       <c r="F7" s="1" t="n">
-        <f aca="false">_xlfn.PERCENTILE.INC(C$2:C$72,0.75)</f>
-        <v>8217.55723905724</v>
+        <f aca="false">_xlfn.PERCENTILE.INC(C$2:C$21,0.75)</f>
+        <v>7668.62777777778</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3257,8 +2364,8 @@
         <v>67</v>
       </c>
       <c r="F8" s="1" t="n">
-        <f aca="false">_xlfn.PERCENTILE.INC(C$2:C$72,0.9)</f>
-        <v>11814.2173913043</v>
+        <f aca="false">_xlfn.PERCENTILE.INC(C$2:C$21,0.9)</f>
+        <v>9856.97940503433</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3415,618 +2522,6 @@
       <c r="C21" s="1" t="n">
         <f aca="false">B21/A21</f>
         <v>10780.7058823529</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B22" s="1" t="n">
-        <v>345345</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <f aca="false">B22/A22</f>
-        <v>7674.33333333333</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B23" s="1" t="n">
-        <v>535357</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <f aca="false">B23/A23</f>
-        <v>15295.9142857143</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B24" s="1" t="n">
-        <v>234242</v>
-      </c>
-      <c r="C24" s="1" t="n">
-        <f aca="false">B24/A24</f>
-        <v>4182.89285714286</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B25" s="1" t="n">
-        <v>345353</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <f aca="false">B25/A25</f>
-        <v>7674.51111111111</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B26" s="1" t="n">
-        <v>342423</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <f aca="false">B26/A26</f>
-        <v>9783.51428571429</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B27" s="1" t="n">
-        <v>235436</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <f aca="false">B27/A27</f>
-        <v>3513.97014925373</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B28" s="1" t="n">
-        <v>435353</v>
-      </c>
-      <c r="C28" s="1" t="n">
-        <f aca="false">B28/A28</f>
-        <v>6697.73846153846</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B29" s="1" t="n">
-        <v>658588</v>
-      </c>
-      <c r="C29" s="1" t="n">
-        <f aca="false">B29/A29</f>
-        <v>12196.0740740741</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B30" s="1" t="n">
-        <v>235655</v>
-      </c>
-      <c r="C30" s="1" t="n">
-        <f aca="false">B30/A30</f>
-        <v>5236.77777777778</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B31" s="1" t="n">
-        <v>455565</v>
-      </c>
-      <c r="C31" s="1" t="n">
-        <f aca="false">B31/A31</f>
-        <v>7008.69230769231</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B32" s="1" t="n">
-        <v>222222</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <f aca="false">B32/A32</f>
-        <v>5167.95348837209</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B33" s="1" t="n">
-        <v>354654</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <f aca="false">B33/A33</f>
-        <v>5293.34328358209</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B34" s="1" t="n">
-        <v>223266</v>
-      </c>
-      <c r="C34" s="1" t="n">
-        <f aca="false">B34/A34</f>
-        <v>6566.64705882353</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B35" s="1" t="n">
-        <v>322266</v>
-      </c>
-      <c r="C35" s="1" t="n">
-        <f aca="false">B35/A35</f>
-        <v>7494.55813953488</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B36" s="1" t="n">
-        <v>323322</v>
-      </c>
-      <c r="C36" s="1" t="n">
-        <f aca="false">B36/A36</f>
-        <v>7184.93333333333</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B37" s="1" t="n">
-        <v>323236</v>
-      </c>
-      <c r="C37" s="1" t="n">
-        <f aca="false">B37/A37</f>
-        <v>7026.86956521739</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B38" s="1" t="n">
-        <v>545444</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <f aca="false">B38/A38</f>
-        <v>11605.1914893617</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B39" s="1" t="n">
-        <v>444546</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <f aca="false">B39/A39</f>
-        <v>8082.65454545455</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B40" s="1" t="n">
-        <v>322322</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <f aca="false">B40/A40</f>
-        <v>5463.08474576271</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B41" s="1" t="n">
-        <v>222222</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <f aca="false">B41/A41</f>
-        <v>3766.47457627119</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B42" s="1" t="n">
-        <v>255464</v>
-      </c>
-      <c r="C42" s="1" t="n">
-        <f aca="false">B42/A42</f>
-        <v>3756.82352941176</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B43" s="1" t="n">
-        <v>565552</v>
-      </c>
-      <c r="C43" s="1" t="n">
-        <f aca="false">B43/A43</f>
-        <v>9585.62711864407</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B44" s="1" t="n">
-        <v>363464</v>
-      </c>
-      <c r="C44" s="1" t="n">
-        <f aca="false">B44/A44</f>
-        <v>5591.75384615385</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B45" s="1" t="n">
-        <v>543454</v>
-      </c>
-      <c r="C45" s="1" t="n">
-        <f aca="false">B45/A45</f>
-        <v>11814.2173913043</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B46" s="1" t="n">
-        <v>352346</v>
-      </c>
-      <c r="C46" s="1" t="n">
-        <f aca="false">B46/A46</f>
-        <v>10067.0285714286</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B47" s="1" t="n">
-        <v>453456</v>
-      </c>
-      <c r="C47" s="1" t="n">
-        <f aca="false">B47/A47</f>
-        <v>13336.9411764706</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B48" s="1" t="n">
-        <v>545633</v>
-      </c>
-      <c r="C48" s="1" t="n">
-        <f aca="false">B48/A48</f>
-        <v>12125.1777777778</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B49" s="1" t="n">
-        <v>335353</v>
-      </c>
-      <c r="C49" s="1" t="n">
-        <f aca="false">B49/A49</f>
-        <v>7290.28260869565</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="B50" s="1" t="n">
-        <v>554564</v>
-      </c>
-      <c r="C50" s="1" t="n">
-        <f aca="false">B50/A50</f>
-        <v>7296.8947368421</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B51" s="1" t="n">
-        <v>551651</v>
-      </c>
-      <c r="C51" s="1" t="n">
-        <f aca="false">B51/A51</f>
-        <v>12258.9111111111</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B52" s="1" t="n">
-        <v>365888</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <f aca="false">B52/A52</f>
-        <v>5629.04615384615</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B53" s="1" t="n">
-        <v>565565</v>
-      </c>
-      <c r="C53" s="1" t="n">
-        <f aca="false">B53/A53</f>
-        <v>12568.1111111111</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B54" s="1" t="n">
-        <v>255686</v>
-      </c>
-      <c r="C54" s="1" t="n">
-        <f aca="false">B54/A54</f>
-        <v>3933.63076923077</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B55" s="1" t="n">
-        <v>226565</v>
-      </c>
-      <c r="C55" s="1" t="n">
-        <f aca="false">B55/A55</f>
-        <v>5034.77777777778</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B56" s="1" t="n">
-        <v>656599</v>
-      </c>
-      <c r="C56" s="1" t="n">
-        <f aca="false">B56/A56</f>
-        <v>13679.1458333333</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B57" s="1" t="n">
-        <v>454455</v>
-      </c>
-      <c r="C57" s="1" t="n">
-        <f aca="false">B57/A57</f>
-        <v>9274.59183673469</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B58" s="1" t="n">
-        <v>415151</v>
-      </c>
-      <c r="C58" s="1" t="n">
-        <f aca="false">B58/A58</f>
-        <v>11220.2972972973</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B59" s="1" t="n">
-        <v>232223</v>
-      </c>
-      <c r="C59" s="1" t="n">
-        <f aca="false">B59/A59</f>
-        <v>4940.91489361702</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B60" s="1" t="n">
-        <v>232232</v>
-      </c>
-      <c r="C60" s="1" t="n">
-        <f aca="false">B60/A60</f>
-        <v>5954.66666666667</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B61" s="1" t="n">
-        <v>232323</v>
-      </c>
-      <c r="C61" s="1" t="n">
-        <f aca="false">B61/A61</f>
-        <v>5280.06818181818</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B62" s="1" t="n">
-        <v>232554</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <f aca="false">B62/A62</f>
-        <v>4844.875</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B63" s="1" t="n">
-        <v>233332</v>
-      </c>
-      <c r="C63" s="1" t="n">
-        <f aca="false">B63/A63</f>
-        <v>3482.5671641791</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B64" s="1" t="n">
-        <v>322555</v>
-      </c>
-      <c r="C64" s="1" t="n">
-        <f aca="false">B64/A64</f>
-        <v>5658.85964912281</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B65" s="1" t="n">
-        <v>245488</v>
-      </c>
-      <c r="C65" s="1" t="n">
-        <f aca="false">B65/A65</f>
-        <v>3776.73846153846</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B66" s="1" t="n">
-        <v>223233</v>
-      </c>
-      <c r="C66" s="1" t="n">
-        <f aca="false">B66/A66</f>
-        <v>4852.89130434783</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B67" s="1" t="n">
-        <v>556555</v>
-      </c>
-      <c r="C67" s="1" t="n">
-        <f aca="false">B67/A67</f>
-        <v>7420.73333333333</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B68" s="1" t="n">
-        <v>226554</v>
-      </c>
-      <c r="C68" s="1" t="n">
-        <f aca="false">B68/A68</f>
-        <v>4119.16363636364</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B69" s="1" t="n">
-        <v>445678</v>
-      </c>
-      <c r="C69" s="1" t="n">
-        <f aca="false">B69/A69</f>
-        <v>8253.2962962963</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B70" s="1" t="n">
-        <v>250000</v>
-      </c>
-      <c r="C70" s="1" t="n">
-        <f aca="false">B70/A70</f>
-        <v>5813.95348837209</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B71" s="1" t="n">
-        <v>280000</v>
-      </c>
-      <c r="C71" s="1" t="n">
-        <f aca="false">B71/A71</f>
-        <v>4179.10447761194</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="B72" s="1" t="n">
-        <v>300000</v>
-      </c>
-      <c r="C72" s="1" t="n">
-        <f aca="false">B72/A72</f>
-        <v>4166.66666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new test sheet. Changed how empty cells for string columns are stored.
</commit_message>
<xml_diff>
--- a/tests/testXlsx.xlsx
+++ b/tests/testXlsx.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Sheet7" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="testAccounts" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
   <si>
     <t xml:space="preserve">Text</t>
   </si>
@@ -230,22 +231,51 @@
   </si>
   <si>
     <t xml:space="preserve">Q90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lic_exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uwagi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zawsze aktualna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">konto zablokowane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$-809]DD/MM/YYYY"/>
     <numFmt numFmtId="168" formatCode="[$-415]GE\nER&quot;al&quot;"/>
-    <numFmt numFmtId="169" formatCode="[$-415]GE\nER&quot;al&quot;"/>
-    <numFmt numFmtId="170" formatCode="[$-415]YYYY\-MM\-DD"/>
-    <numFmt numFmtId="171" formatCode="D\.MM\.YYYY"/>
-    <numFmt numFmtId="172" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="169" formatCode="[$-415]YYYY\-MM\-DD"/>
+    <numFmt numFmtId="170" formatCode="D\.MM\.YYYY"/>
+    <numFmt numFmtId="171" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -373,11 +403,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -389,11 +419,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -421,7 +451,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
   </cols>
@@ -481,7 +511,7 @@
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.39"/>
@@ -969,7 +999,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -992,9 +1022,10 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.13"/>
   </cols>
@@ -1108,7 +1139,7 @@
       <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.58"/>
   </cols>
@@ -1887,7 +1918,7 @@
       <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2218,11 +2249,11 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2308,7 +2339,7 @@
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">_xlfn.PERCENTILE.INC(C$2:C$21,0.25)</f>
-        <v>5065.78947368422</v>
+        <v>5065.78947368421</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2522,6 +2553,77 @@
       <c r="C21" s="1" t="n">
         <f aca="false">B21/A21</f>
         <v>10780.7058823529</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>40816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests for detecting column types during importing of ods files.
</commit_message>
<xml_diff>
--- a/tests/testXlsx.xlsx
+++ b/tests/testXlsx.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -267,15 +267,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="[$-809]DD/MM/YYYY"/>
-    <numFmt numFmtId="168" formatCode="[$-415]GE\nER&quot;al&quot;"/>
-    <numFmt numFmtId="169" formatCode="[$-415]YYYY\-MM\-DD"/>
-    <numFmt numFmtId="170" formatCode="D\.MM\.YYYY"/>
-    <numFmt numFmtId="171" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="167" formatCode="[$-809]dd/mm/yyyy"/>
+    <numFmt numFmtId="168" formatCode="[$-415]ge\ner&quot;al&quot;"/>
+    <numFmt numFmtId="169" formatCode="[$-415]General"/>
+    <numFmt numFmtId="170" formatCode="[$-415]yyyy\-mm\-dd"/>
+    <numFmt numFmtId="171" formatCode="d\.mm\.yyyy"/>
+    <numFmt numFmtId="172" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -374,7 +375,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -403,11 +404,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -419,11 +424,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -448,10 +453,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C2:C5 D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
   </cols>
@@ -508,10 +513,10 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="1" sqref="C2:C5 E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.39"/>
@@ -996,10 +1001,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1018,13 +1023,13 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.13"/>
@@ -1051,14 +1056,14 @@
       <c r="A2" s="7" t="n">
         <v>200000</v>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="8" t="n">
         <v>51</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="8" t="n">
         <f aca="false">A2/B2</f>
         <v>3921.56862745098</v>
       </c>
-      <c r="D2" s="8" t="n">
+      <c r="D2" s="9" t="n">
         <v>40941</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1069,14 +1074,14 @@
       <c r="A3" s="7" t="n">
         <v>200001</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="8" t="n">
         <v>52</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="8" t="n">
         <f aca="false">A3/B3</f>
         <v>3846.17307692308</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="6" t="s">
         <v>40</v>
       </c>
@@ -1085,14 +1090,14 @@
       <c r="A4" s="7" t="n">
         <v>200002</v>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="8" t="n">
         <v>53</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="8" t="n">
         <f aca="false">A4/B4</f>
         <v>3773.62264150943</v>
       </c>
-      <c r="D4" s="8" t="n">
+      <c r="D4" s="9" t="n">
         <v>40943</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -1103,14 +1108,14 @@
       <c r="A5" s="7" t="n">
         <v>200003</v>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="8" t="n">
         <v>54</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="8" t="n">
         <f aca="false">A5/B5</f>
         <v>3703.75925925926</v>
       </c>
-      <c r="D5" s="8" t="n">
+      <c r="D5" s="9" t="n">
         <v>40944</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -1136,10 +1141,10 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="1" sqref="C2:C5 I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.58"/>
   </cols>
@@ -1148,114 +1153,114 @@
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="11" t="n">
+      <c r="B2" s="12" t="n">
         <v>25569</v>
       </c>
-      <c r="C2" s="10" t="n">
+      <c r="C2" s="11" t="n">
         <v>52.21</v>
       </c>
-      <c r="D2" s="10" t="n">
+      <c r="D2" s="11" t="n">
         <v>1.47</v>
       </c>
-      <c r="E2" s="11" t="n">
+      <c r="E2" s="12" t="n">
         <v>25569</v>
       </c>
       <c r="F2" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B2,$E$2)</f>
         <v>0</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="11" t="n">
         <f aca="false">SUM(F2:F16)</f>
         <v>105</v>
       </c>
-      <c r="I2" s="10" t="n">
+      <c r="I2" s="11" t="n">
         <f aca="false">SUM(D2:D16)</f>
         <v>24.76</v>
       </c>
-      <c r="J2" s="10" t="n">
+      <c r="J2" s="11" t="n">
         <f aca="false">F2*F2</f>
         <v>0</v>
       </c>
-      <c r="K2" s="10" t="n">
+      <c r="K2" s="11" t="n">
         <f aca="false">C2*C2</f>
         <v>2725.8841</v>
       </c>
-      <c r="L2" s="10" t="n">
+      <c r="L2" s="11" t="n">
         <f aca="false">F2*C2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="12" t="n">
+      <c r="B3" s="13" t="n">
         <f aca="false">B2+1</f>
         <v>25570</v>
       </c>
-      <c r="C3" s="10" t="n">
+      <c r="C3" s="11" t="n">
         <v>53.12</v>
       </c>
-      <c r="D3" s="10" t="n">
+      <c r="D3" s="11" t="n">
         <v>1.5</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B3,$E$2)</f>
         <v>1</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="10" t="n">
+      <c r="H3" s="11" t="n">
         <f aca="false">SUM(C2:C16)</f>
         <v>931.17</v>
       </c>
-      <c r="I3" s="10" t="n">
+      <c r="I3" s="11" t="n">
         <f aca="false">SUM(C2:C16)</f>
         <v>931.17</v>
       </c>
-      <c r="J3" s="10" t="n">
+      <c r="J3" s="11" t="n">
         <f aca="false">F3*F3</f>
         <v>1</v>
       </c>
-      <c r="K3" s="10" t="n">
+      <c r="K3" s="11" t="n">
         <f aca="false">C3*C3</f>
         <v>2821.7344</v>
       </c>
-      <c r="L3" s="10" t="n">
+      <c r="L3" s="11" t="n">
         <f aca="false">F3*C3</f>
         <v>53.12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="12" t="n">
+      <c r="B4" s="13" t="n">
         <f aca="false">B3+1</f>
         <v>25571</v>
       </c>
-      <c r="C4" s="10" t="n">
+      <c r="C4" s="11" t="n">
         <v>54.48</v>
       </c>
-      <c r="D4" s="10" t="n">
+      <c r="D4" s="11" t="n">
         <v>1.52</v>
       </c>
       <c r="F4" s="1" t="n">
@@ -1273,28 +1278,28 @@
         <f aca="false">SUM(J18:J32)</f>
         <v>41.0532</v>
       </c>
-      <c r="J4" s="10" t="n">
+      <c r="J4" s="11" t="n">
         <f aca="false">F4*F4</f>
         <v>4</v>
       </c>
-      <c r="K4" s="10" t="n">
+      <c r="K4" s="11" t="n">
         <f aca="false">C4*C4</f>
         <v>2968.0704</v>
       </c>
-      <c r="L4" s="10" t="n">
+      <c r="L4" s="11" t="n">
         <f aca="false">F4*C4</f>
         <v>108.96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="12" t="n">
+      <c r="B5" s="13" t="n">
         <f aca="false">B4+1</f>
         <v>25572</v>
       </c>
-      <c r="C5" s="10" t="n">
+      <c r="C5" s="11" t="n">
         <v>55.84</v>
       </c>
-      <c r="D5" s="10" t="n">
+      <c r="D5" s="11" t="n">
         <v>1.55</v>
       </c>
       <c r="F5" s="1" t="n">
@@ -1312,28 +1317,28 @@
         <f aca="false">SUM(K18:K32)</f>
         <v>58498.5439</v>
       </c>
-      <c r="J5" s="10" t="n">
+      <c r="J5" s="11" t="n">
         <f aca="false">F5*F5</f>
         <v>9</v>
       </c>
-      <c r="K5" s="10" t="n">
+      <c r="K5" s="11" t="n">
         <f aca="false">C5*C5</f>
         <v>3118.1056</v>
       </c>
-      <c r="L5" s="10" t="n">
+      <c r="L5" s="11" t="n">
         <f aca="false">F5*C5</f>
         <v>167.52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="12" t="n">
+      <c r="B6" s="13" t="n">
         <f aca="false">B5+1</f>
         <v>25573</v>
       </c>
-      <c r="C6" s="10" t="n">
+      <c r="C6" s="11" t="n">
         <v>57.2</v>
       </c>
-      <c r="D6" s="10" t="n">
+      <c r="D6" s="11" t="n">
         <v>1.57</v>
       </c>
       <c r="F6" s="1" t="n">
@@ -1351,28 +1356,28 @@
         <f aca="false">SUM(L18:L32)</f>
         <v>1548.2453</v>
       </c>
-      <c r="J6" s="10" t="n">
+      <c r="J6" s="11" t="n">
         <f aca="false">F6*F6</f>
         <v>16</v>
       </c>
-      <c r="K6" s="10" t="n">
+      <c r="K6" s="11" t="n">
         <f aca="false">C6*C6</f>
         <v>3271.84</v>
       </c>
-      <c r="L6" s="10" t="n">
+      <c r="L6" s="11" t="n">
         <f aca="false">F6*C6</f>
         <v>228.8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="12" t="n">
+      <c r="B7" s="13" t="n">
         <f aca="false">B6+1</f>
         <v>25574</v>
       </c>
-      <c r="C7" s="10" t="n">
+      <c r="C7" s="11" t="n">
         <v>58.57</v>
       </c>
-      <c r="D7" s="10" t="n">
+      <c r="D7" s="11" t="n">
         <v>1.6</v>
       </c>
       <c r="F7" s="1" t="n">
@@ -1388,28 +1393,28 @@
       <c r="I7" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="J7" s="10" t="n">
+      <c r="J7" s="11" t="n">
         <f aca="false">F7*F7</f>
         <v>25</v>
       </c>
-      <c r="K7" s="10" t="n">
+      <c r="K7" s="11" t="n">
         <f aca="false">C7*C7</f>
         <v>3430.4449</v>
       </c>
-      <c r="L7" s="10" t="n">
+      <c r="L7" s="11" t="n">
         <f aca="false">F7*C7</f>
         <v>292.85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="12" t="n">
+      <c r="B8" s="13" t="n">
         <f aca="false">B7+1</f>
         <v>25575</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="11" t="n">
         <v>59.93</v>
       </c>
-      <c r="D8" s="10" t="n">
+      <c r="D8" s="11" t="n">
         <v>1.63</v>
       </c>
       <c r="F8" s="1" t="n">
@@ -1427,28 +1432,28 @@
         <f aca="false">(I7*I6-I2*I3)/(I7*I4-I2*I2)</f>
         <v>61.2721865421088</v>
       </c>
-      <c r="J8" s="10" t="n">
+      <c r="J8" s="11" t="n">
         <f aca="false">F8*F8</f>
         <v>36</v>
       </c>
-      <c r="K8" s="10" t="n">
+      <c r="K8" s="11" t="n">
         <f aca="false">C8*C8</f>
         <v>3591.6049</v>
       </c>
-      <c r="L8" s="10" t="n">
+      <c r="L8" s="11" t="n">
         <f aca="false">F8*C8</f>
         <v>359.58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="12" t="n">
+      <c r="B9" s="13" t="n">
         <f aca="false">B8+1</f>
         <v>25576</v>
       </c>
-      <c r="C9" s="10" t="n">
+      <c r="C9" s="11" t="n">
         <v>61.29</v>
       </c>
-      <c r="D9" s="10" t="n">
+      <c r="D9" s="11" t="n">
         <v>1.65</v>
       </c>
       <c r="F9" s="1" t="n">
@@ -1466,56 +1471,56 @@
         <f aca="false">1/I7*I3-I8*1/I7*I2</f>
         <v>-39.0619559188409</v>
       </c>
-      <c r="J9" s="10" t="n">
+      <c r="J9" s="11" t="n">
         <f aca="false">F9*F9</f>
         <v>49</v>
       </c>
-      <c r="K9" s="10" t="n">
+      <c r="K9" s="11" t="n">
         <f aca="false">C9*C9</f>
         <v>3756.4641</v>
       </c>
-      <c r="L9" s="10" t="n">
+      <c r="L9" s="11" t="n">
         <f aca="false">F9*C9</f>
         <v>429.03</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12" t="n">
+      <c r="B10" s="13" t="n">
         <f aca="false">B9+1</f>
         <v>25577</v>
       </c>
-      <c r="C10" s="10" t="n">
+      <c r="C10" s="11" t="n">
         <v>63.11</v>
       </c>
-      <c r="D10" s="10" t="n">
+      <c r="D10" s="11" t="n">
         <v>1.68</v>
       </c>
       <c r="F10" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B10,$E$2)</f>
         <v>8</v>
       </c>
-      <c r="J10" s="10" t="n">
+      <c r="J10" s="11" t="n">
         <f aca="false">F10*F10</f>
         <v>64</v>
       </c>
-      <c r="K10" s="10" t="n">
+      <c r="K10" s="11" t="n">
         <f aca="false">C10*C10</f>
         <v>3982.8721</v>
       </c>
-      <c r="L10" s="10" t="n">
+      <c r="L10" s="11" t="n">
         <f aca="false">F10*C10</f>
         <v>504.88</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="n">
+      <c r="B11" s="13" t="n">
         <f aca="false">B10+1</f>
         <v>25578</v>
       </c>
-      <c r="C11" s="10" t="n">
+      <c r="C11" s="11" t="n">
         <v>64.47</v>
       </c>
-      <c r="D11" s="10" t="n">
+      <c r="D11" s="11" t="n">
         <v>1.7</v>
       </c>
       <c r="F11" s="1" t="n">
@@ -1525,155 +1530,155 @@
       <c r="H11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="10" t="n">
+      <c r="J11" s="11" t="n">
         <f aca="false">F11*F11</f>
         <v>81</v>
       </c>
-      <c r="K11" s="10" t="n">
+      <c r="K11" s="11" t="n">
         <f aca="false">C11*C11</f>
         <v>4156.3809</v>
       </c>
-      <c r="L11" s="10" t="n">
+      <c r="L11" s="11" t="n">
         <f aca="false">F11*C11</f>
         <v>580.23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="n">
+      <c r="B12" s="13" t="n">
         <f aca="false">B11+1</f>
         <v>25579</v>
       </c>
-      <c r="C12" s="10" t="n">
+      <c r="C12" s="11" t="n">
         <v>66.28</v>
       </c>
-      <c r="D12" s="10" t="n">
+      <c r="D12" s="11" t="n">
         <v>1.73</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B12,$E$2)</f>
         <v>10</v>
       </c>
-      <c r="J12" s="10" t="n">
+      <c r="J12" s="11" t="n">
         <f aca="false">F12*F12</f>
         <v>100</v>
       </c>
-      <c r="K12" s="10" t="n">
+      <c r="K12" s="11" t="n">
         <f aca="false">C12*C12</f>
         <v>4393.0384</v>
       </c>
-      <c r="L12" s="10" t="n">
+      <c r="L12" s="11" t="n">
         <f aca="false">F12*C12</f>
         <v>662.8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="n">
+      <c r="B13" s="13" t="n">
         <f aca="false">B12+1</f>
         <v>25580</v>
       </c>
-      <c r="C13" s="10" t="n">
+      <c r="C13" s="11" t="n">
         <v>68.1</v>
       </c>
-      <c r="D13" s="10" t="n">
+      <c r="D13" s="11" t="n">
         <v>1.75</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B13,$E$2)</f>
         <v>11</v>
       </c>
-      <c r="J13" s="10" t="n">
+      <c r="J13" s="11" t="n">
         <f aca="false">F13*F13</f>
         <v>121</v>
       </c>
-      <c r="K13" s="10" t="n">
+      <c r="K13" s="11" t="n">
         <f aca="false">C13*C13</f>
         <v>4637.61</v>
       </c>
-      <c r="L13" s="10" t="n">
+      <c r="L13" s="11" t="n">
         <f aca="false">F13*C13</f>
         <v>749.1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="n">
+      <c r="B14" s="13" t="n">
         <f aca="false">B13+1</f>
         <v>25581</v>
       </c>
-      <c r="C14" s="10" t="n">
+      <c r="C14" s="11" t="n">
         <v>69.92</v>
       </c>
-      <c r="D14" s="10" t="n">
+      <c r="D14" s="11" t="n">
         <v>1.78</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B14,$E$2)</f>
         <v>12</v>
       </c>
-      <c r="J14" s="10" t="n">
+      <c r="J14" s="11" t="n">
         <f aca="false">F14*F14</f>
         <v>144</v>
       </c>
-      <c r="K14" s="10" t="n">
+      <c r="K14" s="11" t="n">
         <f aca="false">C14*C14</f>
         <v>4888.8064</v>
       </c>
-      <c r="L14" s="10" t="n">
+      <c r="L14" s="11" t="n">
         <f aca="false">F14*C14</f>
         <v>839.04</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="n">
+      <c r="B15" s="13" t="n">
         <f aca="false">B14+1</f>
         <v>25582</v>
       </c>
-      <c r="C15" s="10" t="n">
+      <c r="C15" s="11" t="n">
         <v>72.19</v>
       </c>
-      <c r="D15" s="10" t="n">
+      <c r="D15" s="11" t="n">
         <v>1.8</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B15,$E$2)</f>
         <v>13</v>
       </c>
-      <c r="J15" s="10" t="n">
+      <c r="J15" s="11" t="n">
         <f aca="false">F15*F15</f>
         <v>169</v>
       </c>
-      <c r="K15" s="10" t="n">
+      <c r="K15" s="11" t="n">
         <f aca="false">C15*C15</f>
         <v>5211.3961</v>
       </c>
-      <c r="L15" s="10" t="n">
+      <c r="L15" s="11" t="n">
         <f aca="false">F15*C15</f>
         <v>938.47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="n">
+      <c r="B16" s="13" t="n">
         <f aca="false">B15+1</f>
         <v>25583</v>
       </c>
-      <c r="C16" s="10" t="n">
+      <c r="C16" s="11" t="n">
         <v>74.46</v>
       </c>
-      <c r="D16" s="10" t="n">
+      <c r="D16" s="11" t="n">
         <v>1.83</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">_xlfn.DAYS(B16,$E$2)</f>
         <v>14</v>
       </c>
-      <c r="J16" s="10" t="n">
+      <c r="J16" s="11" t="n">
         <f aca="false">F16*F16</f>
         <v>196</v>
       </c>
-      <c r="K16" s="10" t="n">
+      <c r="K16" s="11" t="n">
         <f aca="false">C16*C16</f>
         <v>5544.2916</v>
       </c>
-      <c r="L16" s="10" t="n">
+      <c r="L16" s="11" t="n">
         <f aca="false">F16*C16</f>
         <v>1042.44</v>
       </c>
@@ -1683,7 +1688,7 @@
         <f aca="false">D2*D2</f>
         <v>2.1609</v>
       </c>
-      <c r="K18" s="10" t="n">
+      <c r="K18" s="11" t="n">
         <f aca="false">C2*C2</f>
         <v>2725.8841</v>
       </c>
@@ -1697,7 +1702,7 @@
         <f aca="false">D3*D3</f>
         <v>2.25</v>
       </c>
-      <c r="K19" s="10" t="n">
+      <c r="K19" s="11" t="n">
         <f aca="false">C3*C3</f>
         <v>2821.7344</v>
       </c>
@@ -1711,7 +1716,7 @@
         <f aca="false">D4*D4</f>
         <v>2.3104</v>
       </c>
-      <c r="K20" s="10" t="n">
+      <c r="K20" s="11" t="n">
         <f aca="false">C4*C4</f>
         <v>2968.0704</v>
       </c>
@@ -1725,7 +1730,7 @@
         <f aca="false">D5*D5</f>
         <v>2.4025</v>
       </c>
-      <c r="K21" s="10" t="n">
+      <c r="K21" s="11" t="n">
         <f aca="false">C5*C5</f>
         <v>3118.1056</v>
       </c>
@@ -1739,7 +1744,7 @@
         <f aca="false">D6*D6</f>
         <v>2.4649</v>
       </c>
-      <c r="K22" s="10" t="n">
+      <c r="K22" s="11" t="n">
         <f aca="false">C6*C6</f>
         <v>3271.84</v>
       </c>
@@ -1753,7 +1758,7 @@
         <f aca="false">D7*D7</f>
         <v>2.56</v>
       </c>
-      <c r="K23" s="10" t="n">
+      <c r="K23" s="11" t="n">
         <f aca="false">C7*C7</f>
         <v>3430.4449</v>
       </c>
@@ -1767,7 +1772,7 @@
         <f aca="false">D8*D8</f>
         <v>2.6569</v>
       </c>
-      <c r="K24" s="10" t="n">
+      <c r="K24" s="11" t="n">
         <f aca="false">C8*C8</f>
         <v>3591.6049</v>
       </c>
@@ -1777,19 +1782,19 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
       <c r="J25" s="1" t="n">
         <f aca="false">D9*D9</f>
         <v>2.7225</v>
       </c>
-      <c r="K25" s="10" t="n">
+      <c r="K25" s="11" t="n">
         <f aca="false">C9*C9</f>
         <v>3756.4641</v>
       </c>
@@ -1803,7 +1808,7 @@
         <f aca="false">D10*D10</f>
         <v>2.8224</v>
       </c>
-      <c r="K26" s="10" t="n">
+      <c r="K26" s="11" t="n">
         <f aca="false">C10*C10</f>
         <v>3982.8721</v>
       </c>
@@ -1817,7 +1822,7 @@
         <f aca="false">D11*D11</f>
         <v>2.89</v>
       </c>
-      <c r="K27" s="10" t="n">
+      <c r="K27" s="11" t="n">
         <f aca="false">C11*C11</f>
         <v>4156.3809</v>
       </c>
@@ -1831,7 +1836,7 @@
         <f aca="false">D12*D12</f>
         <v>2.9929</v>
       </c>
-      <c r="K28" s="10" t="n">
+      <c r="K28" s="11" t="n">
         <f aca="false">C12*C12</f>
         <v>4393.0384</v>
       </c>
@@ -1845,7 +1850,7 @@
         <f aca="false">D13*D13</f>
         <v>3.0625</v>
       </c>
-      <c r="K29" s="10" t="n">
+      <c r="K29" s="11" t="n">
         <f aca="false">C13*C13</f>
         <v>4637.61</v>
       </c>
@@ -1859,7 +1864,7 @@
         <f aca="false">D14*D14</f>
         <v>3.1684</v>
       </c>
-      <c r="K30" s="10" t="n">
+      <c r="K30" s="11" t="n">
         <f aca="false">C14*C14</f>
         <v>4888.8064</v>
       </c>
@@ -1873,7 +1878,7 @@
         <f aca="false">D15*D15</f>
         <v>3.24</v>
       </c>
-      <c r="K31" s="10" t="n">
+      <c r="K31" s="11" t="n">
         <f aca="false">C15*C15</f>
         <v>5211.3961</v>
       </c>
@@ -1887,7 +1892,7 @@
         <f aca="false">D16*D16</f>
         <v>3.3489</v>
       </c>
-      <c r="K32" s="10" t="n">
+      <c r="K32" s="11" t="n">
         <f aca="false">C16*C16</f>
         <v>5544.2916</v>
       </c>
@@ -1915,10 +1920,10 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topLeft" activeCell="A27" activeCellId="1" sqref="C2:C5 A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2250,10 +2255,10 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="1" sqref="C2:C5 A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2573,11 +2578,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="1" sqref="C2:C5 F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
Additional test case added. Rework of import classes.
</commit_message>
<xml_diff>
--- a/tests/testXlsx.xlsx
+++ b/tests/testXlsx.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,8 @@
     <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Sheet7" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="testAccounts" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Sheet9" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="testAccounts" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
   <si>
     <t xml:space="preserve">Text</t>
   </si>
@@ -231,6 +232,18 @@
   </si>
   <si>
     <t xml:space="preserve">Q90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">second</t>
+  </si>
+  <si>
+    <t xml:space="preserve">third</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
   </si>
   <si>
     <t xml:space="preserve">user</t>
@@ -273,7 +286,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$-809]dd/mm/yyyy"/>
     <numFmt numFmtId="168" formatCode="[$-415]ge\ner&quot;al&quot;"/>
-    <numFmt numFmtId="169" formatCode="[$-415]General"/>
+    <numFmt numFmtId="169" formatCode="[$-415]ge\ner&quot;al&quot;"/>
     <numFmt numFmtId="170" formatCode="[$-415]yyyy\-mm\-dd"/>
     <numFmt numFmtId="171" formatCode="d\.mm\.yyyy"/>
     <numFmt numFmtId="172" formatCode="dd/mm/yy"/>
@@ -453,10 +466,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C2:C5 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
   </cols>
@@ -513,10 +526,10 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="1" sqref="C2:C5 E6"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.39"/>
@@ -1001,10 +1014,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1023,11 +1036,11 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.7"/>
@@ -1141,10 +1154,10 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="1" sqref="C2:C5 I9"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.58"/>
   </cols>
@@ -1920,10 +1933,10 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="1" sqref="C2:C5 A27"/>
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2255,10 +2268,10 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="1" sqref="C2:C5 A22"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2576,56 +2589,112 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="1" sqref="C2:C5 F17"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>73</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>40816</v>

</xml_diff>

<commit_message>
New test case added for spreadsheet importing.
</commit_message>
<xml_diff>
--- a/tests/testXlsx.xlsx
+++ b/tests/testXlsx.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
   <si>
     <t xml:space="preserve">Text</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t xml:space="preserve">third</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fourth</t>
   </si>
   <si>
     <t xml:space="preserve">s</t>
@@ -280,7 +283,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
@@ -290,6 +293,7 @@
     <numFmt numFmtId="170" formatCode="[$-415]yyyy\-mm\-dd"/>
     <numFmt numFmtId="171" formatCode="d\.mm\.yyyy"/>
     <numFmt numFmtId="172" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="173" formatCode="yyyy\-mm\-dd\ hh:mm"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -388,7 +392,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -445,6 +449,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2589,13 +2597,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -2604,28 +2616,34 @@
       <c r="C1" s="0" t="s">
         <v>69</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="14" t="n">
+        <v>40909.5163657407</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="C2" s="0" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>67</v>
       </c>
     </row>
@@ -2655,46 +2673,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>40816</v>

</xml_diff>